<commit_message>
Projektplan v1.0, Kravspec v2.0
Se rubrik
</commit_message>
<xml_diff>
--- a/docs/projektgrupp6_tidsplan.xlsx
+++ b/docs/projektgrupp6_tidsplan.xlsx
@@ -1,27 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20904"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20919"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\TNE085\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\TNE085\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_3815019EB98DA7E9140BA46B124DD5CBD053FB07" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{40CFA809-CE5F-449A-9D97-6C41D4E01605}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="15180" windowHeight="8580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17700" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Basplan" sheetId="1" r:id="rId1"/>
     <sheet name="Summering TID" sheetId="5" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179020"/>
+  <calcPr calcId="179020" calcCompleted="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="57">
   <si>
     <t>PLANERING</t>
   </si>
@@ -53,9 +53,6 @@
     <t>Version:</t>
   </si>
   <si>
-    <t>1.0</t>
-  </si>
-  <si>
     <t>Kurs:</t>
   </si>
   <si>
@@ -191,19 +188,7 @@
     <t>Su</t>
   </si>
   <si>
-    <t>Anna Andersson</t>
-  </si>
-  <si>
-    <t>Kalle Karlsson</t>
-  </si>
-  <si>
-    <t>Olle Olsson</t>
-  </si>
-  <si>
-    <t>Pelle Perssson</t>
-  </si>
-  <si>
-    <t>Stina Svensson</t>
+    <t>Gustav Palmqvist</t>
   </si>
   <si>
     <t xml:space="preserve">Summa antal timmar:  </t>
@@ -1100,41 +1085,22 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1142,119 +1108,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1267,12 +1120,176 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1318,38 +1335,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1638,8 +1623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="T43" sqref="T43"/>
+    <sheetView workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1656,108 +1641,109 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" s="15" customFormat="1" ht="18">
-      <c r="A1" s="111" t="s">
+      <c r="A1" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="112"/>
-      <c r="C1" s="112"/>
-      <c r="D1" s="112"/>
-      <c r="E1" s="112"/>
-      <c r="F1" s="112"/>
-      <c r="G1" s="112"/>
-      <c r="H1" s="112"/>
-      <c r="I1" s="112"/>
-      <c r="J1" s="112"/>
-      <c r="K1" s="112"/>
-      <c r="L1" s="112"/>
-      <c r="M1" s="112"/>
-      <c r="N1" s="112"/>
-      <c r="O1" s="112"/>
-      <c r="P1" s="112"/>
-      <c r="Q1" s="112"/>
-      <c r="R1" s="112"/>
-      <c r="S1" s="112"/>
-      <c r="T1" s="112"/>
-      <c r="U1" s="112"/>
-      <c r="V1" s="112"/>
-      <c r="W1" s="112"/>
-      <c r="X1" s="112"/>
-      <c r="Y1" s="112"/>
-      <c r="Z1" s="112"/>
-      <c r="AA1" s="112"/>
-      <c r="AB1" s="112"/>
-      <c r="AC1" s="112"/>
-      <c r="AD1" s="112"/>
-      <c r="AE1" s="113"/>
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="73"/>
+      <c r="J1" s="73"/>
+      <c r="K1" s="73"/>
+      <c r="L1" s="73"/>
+      <c r="M1" s="73"/>
+      <c r="N1" s="73"/>
+      <c r="O1" s="73"/>
+      <c r="P1" s="73"/>
+      <c r="Q1" s="73"/>
+      <c r="R1" s="73"/>
+      <c r="S1" s="73"/>
+      <c r="T1" s="73"/>
+      <c r="U1" s="73"/>
+      <c r="V1" s="73"/>
+      <c r="W1" s="73"/>
+      <c r="X1" s="73"/>
+      <c r="Y1" s="73"/>
+      <c r="Z1" s="73"/>
+      <c r="AA1" s="73"/>
+      <c r="AB1" s="73"/>
+      <c r="AC1" s="73"/>
+      <c r="AD1" s="73"/>
+      <c r="AE1" s="74"/>
     </row>
     <row r="2" spans="1:31" s="15" customFormat="1" ht="18.75" thickBot="1">
-      <c r="A2" s="80" t="s">
+      <c r="A2" s="93" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="81"/>
+      <c r="B2" s="94"/>
       <c r="C2" s="54"/>
-      <c r="D2" s="114" t="s">
+      <c r="D2" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="114"/>
-      <c r="F2" s="114"/>
-      <c r="G2" s="114"/>
-      <c r="H2" s="114"/>
-      <c r="I2" s="114"/>
-      <c r="J2" s="114"/>
-      <c r="K2" s="114"/>
-      <c r="L2" s="114"/>
-      <c r="M2" s="114"/>
-      <c r="N2" s="114"/>
-      <c r="O2" s="114"/>
-      <c r="P2" s="114"/>
-      <c r="Q2" s="114"/>
-      <c r="R2" s="114"/>
-      <c r="S2" s="114"/>
-      <c r="T2" s="114"/>
-      <c r="U2" s="114"/>
-      <c r="V2" s="114"/>
-      <c r="W2" s="114"/>
-      <c r="X2" s="114"/>
-      <c r="Y2" s="114"/>
-      <c r="Z2" s="114"/>
-      <c r="AA2" s="114"/>
-      <c r="AB2" s="114"/>
-      <c r="AC2" s="114"/>
-      <c r="AD2" s="114"/>
-      <c r="AE2" s="115"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="75"/>
+      <c r="K2" s="75"/>
+      <c r="L2" s="75"/>
+      <c r="M2" s="75"/>
+      <c r="N2" s="75"/>
+      <c r="O2" s="75"/>
+      <c r="P2" s="75"/>
+      <c r="Q2" s="75"/>
+      <c r="R2" s="75"/>
+      <c r="S2" s="75"/>
+      <c r="T2" s="75"/>
+      <c r="U2" s="75"/>
+      <c r="V2" s="75"/>
+      <c r="W2" s="75"/>
+      <c r="X2" s="75"/>
+      <c r="Y2" s="75"/>
+      <c r="Z2" s="75"/>
+      <c r="AA2" s="75"/>
+      <c r="AB2" s="75"/>
+      <c r="AC2" s="75"/>
+      <c r="AD2" s="75"/>
+      <c r="AE2" s="76"/>
     </row>
     <row r="3" spans="1:31" ht="15.75">
-      <c r="A3" s="78" t="s">
+      <c r="A3" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="79"/>
+      <c r="B3" s="92"/>
       <c r="C3" s="13"/>
-      <c r="D3" s="99" t="s">
+      <c r="D3" s="97" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="99"/>
-      <c r="F3" s="100"/>
-      <c r="G3" s="78" t="s">
+      <c r="E3" s="97"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="91" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="79"/>
-      <c r="I3" s="88">
-        <v>43353</v>
-      </c>
-      <c r="J3" s="88"/>
-      <c r="K3" s="88"/>
-      <c r="L3" s="88"/>
-      <c r="M3" s="88"/>
-      <c r="N3" s="88"/>
-      <c r="O3" s="89"/>
-      <c r="P3" s="78" t="s">
+      <c r="H3" s="92"/>
+      <c r="I3" s="116">
+        <f ca="1">NOW()</f>
+        <v>43366.704446064818</v>
+      </c>
+      <c r="J3" s="116"/>
+      <c r="K3" s="116"/>
+      <c r="L3" s="116"/>
+      <c r="M3" s="116"/>
+      <c r="N3" s="116"/>
+      <c r="O3" s="117"/>
+      <c r="P3" s="91" t="s">
         <v>6</v>
       </c>
-      <c r="Q3" s="79"/>
-      <c r="R3" s="79"/>
-      <c r="S3" s="79"/>
-      <c r="T3" s="79"/>
+      <c r="Q3" s="92"/>
+      <c r="R3" s="92"/>
+      <c r="S3" s="92"/>
+      <c r="T3" s="92"/>
       <c r="U3" s="5"/>
       <c r="V3" s="5"/>
       <c r="W3" s="5"/>
@@ -1771,29 +1757,29 @@
       <c r="AE3" s="4"/>
     </row>
     <row r="4" spans="1:31" ht="15.75">
-      <c r="A4" s="84" t="s">
+      <c r="A4" s="105" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="85"/>
+      <c r="B4" s="106"/>
       <c r="C4" s="13"/>
-      <c r="D4" s="101" t="s">
+      <c r="D4" s="99" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="101"/>
-      <c r="F4" s="102"/>
-      <c r="G4" s="84" t="s">
+      <c r="E4" s="99"/>
+      <c r="F4" s="100"/>
+      <c r="G4" s="105" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="85"/>
-      <c r="I4" s="90" t="s">
-        <v>10</v>
-      </c>
-      <c r="J4" s="90"/>
-      <c r="K4" s="90"/>
-      <c r="L4" s="90"/>
-      <c r="M4" s="90"/>
-      <c r="N4" s="90"/>
-      <c r="O4" s="91"/>
+      <c r="H4" s="106"/>
+      <c r="I4" s="118">
+        <v>1</v>
+      </c>
+      <c r="J4" s="118"/>
+      <c r="K4" s="118"/>
+      <c r="L4" s="118"/>
+      <c r="M4" s="118"/>
+      <c r="N4" s="118"/>
+      <c r="O4" s="119"/>
       <c r="P4" s="3"/>
       <c r="Q4" s="14"/>
       <c r="R4" s="14"/>
@@ -1812,29 +1798,29 @@
       <c r="AE4" s="4"/>
     </row>
     <row r="5" spans="1:31" ht="16.5" thickBot="1">
-      <c r="A5" s="86" t="s">
+      <c r="A5" s="103" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="104"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="101" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="87"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="103" t="s">
+      <c r="E5" s="101"/>
+      <c r="F5" s="102"/>
+      <c r="G5" s="103" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="103"/>
-      <c r="F5" s="104"/>
-      <c r="G5" s="86" t="s">
+      <c r="H5" s="104"/>
+      <c r="I5" s="120" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="87"/>
-      <c r="I5" s="92" t="s">
-        <v>14</v>
-      </c>
-      <c r="J5" s="92"/>
-      <c r="K5" s="92"/>
-      <c r="L5" s="92"/>
-      <c r="M5" s="92"/>
-      <c r="N5" s="92"/>
-      <c r="O5" s="93"/>
+      <c r="J5" s="120"/>
+      <c r="K5" s="120"/>
+      <c r="L5" s="120"/>
+      <c r="M5" s="120"/>
+      <c r="N5" s="120"/>
+      <c r="O5" s="121"/>
       <c r="P5" s="3"/>
       <c r="Q5" s="5"/>
       <c r="R5" s="5"/>
@@ -1853,61 +1839,61 @@
       <c r="AE5" s="4"/>
     </row>
     <row r="6" spans="1:31" s="2" customFormat="1" ht="16.5" thickBot="1">
-      <c r="A6" s="82" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="83"/>
-      <c r="C6" s="83"/>
-      <c r="D6" s="83"/>
+      <c r="A6" s="77" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="78"/>
+      <c r="C6" s="78"/>
+      <c r="D6" s="78"/>
       <c r="E6" s="1"/>
       <c r="F6" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="H6" s="77" t="s">
         <v>17</v>
       </c>
-      <c r="H6" s="82" t="s">
-        <v>18</v>
-      </c>
-      <c r="I6" s="83"/>
-      <c r="J6" s="83"/>
-      <c r="K6" s="83"/>
-      <c r="L6" s="83"/>
-      <c r="M6" s="83"/>
-      <c r="N6" s="83"/>
-      <c r="O6" s="83"/>
-      <c r="P6" s="83"/>
-      <c r="Q6" s="83"/>
-      <c r="R6" s="83"/>
-      <c r="S6" s="83"/>
-      <c r="T6" s="83"/>
-      <c r="U6" s="83"/>
-      <c r="V6" s="83"/>
-      <c r="W6" s="83"/>
-      <c r="X6" s="83"/>
-      <c r="Y6" s="83"/>
-      <c r="Z6" s="83"/>
-      <c r="AA6" s="83"/>
-      <c r="AB6" s="83"/>
-      <c r="AC6" s="83"/>
-      <c r="AD6" s="83"/>
-      <c r="AE6" s="116"/>
+      <c r="I6" s="78"/>
+      <c r="J6" s="78"/>
+      <c r="K6" s="78"/>
+      <c r="L6" s="78"/>
+      <c r="M6" s="78"/>
+      <c r="N6" s="78"/>
+      <c r="O6" s="78"/>
+      <c r="P6" s="78"/>
+      <c r="Q6" s="78"/>
+      <c r="R6" s="78"/>
+      <c r="S6" s="78"/>
+      <c r="T6" s="78"/>
+      <c r="U6" s="78"/>
+      <c r="V6" s="78"/>
+      <c r="W6" s="78"/>
+      <c r="X6" s="78"/>
+      <c r="Y6" s="78"/>
+      <c r="Z6" s="78"/>
+      <c r="AA6" s="78"/>
+      <c r="AB6" s="78"/>
+      <c r="AC6" s="78"/>
+      <c r="AD6" s="78"/>
+      <c r="AE6" s="79"/>
     </row>
     <row r="7" spans="1:31" ht="13.5" thickBot="1">
       <c r="A7" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="80" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="117" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="118"/>
-      <c r="D7" s="119"/>
+      <c r="C7" s="81"/>
+      <c r="D7" s="82"/>
       <c r="E7" s="8"/>
       <c r="F7" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="9" t="s">
         <v>21</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>22</v>
       </c>
       <c r="H7" s="10">
         <v>36</v>
@@ -1984,17 +1970,17 @@
       <c r="A8" s="11">
         <v>1</v>
       </c>
-      <c r="B8" s="105" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="106"/>
-      <c r="D8" s="107"/>
+      <c r="B8" s="107" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="108"/>
+      <c r="D8" s="109"/>
       <c r="E8" s="18"/>
       <c r="F8" s="19">
         <v>20</v>
       </c>
       <c r="G8" s="31" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H8" s="69"/>
       <c r="I8" s="70"/>
@@ -2025,17 +2011,17 @@
       <c r="A9" s="11">
         <v>2</v>
       </c>
-      <c r="B9" s="94" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="95"/>
-      <c r="D9" s="96"/>
+      <c r="B9" s="86" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="87"/>
+      <c r="D9" s="88"/>
       <c r="E9" s="21"/>
       <c r="F9" s="22">
         <v>16</v>
       </c>
       <c r="G9" s="31" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H9" s="71"/>
       <c r="I9" s="68"/>
@@ -2066,17 +2052,17 @@
       <c r="A10" s="11">
         <v>3</v>
       </c>
-      <c r="B10" s="94" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="95"/>
-      <c r="D10" s="96"/>
+      <c r="B10" s="86" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="87"/>
+      <c r="D10" s="88"/>
       <c r="E10" s="21"/>
       <c r="F10" s="22">
         <v>8</v>
       </c>
       <c r="G10" s="31" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H10" s="71"/>
       <c r="I10" s="68"/>
@@ -2107,17 +2093,17 @@
       <c r="A11" s="11">
         <v>4</v>
       </c>
-      <c r="B11" s="94" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="95"/>
-      <c r="D11" s="96"/>
+      <c r="B11" s="86" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="87"/>
+      <c r="D11" s="88"/>
       <c r="E11" s="21"/>
       <c r="F11" s="22">
         <v>8</v>
       </c>
       <c r="G11" s="31" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H11" s="23"/>
       <c r="I11" s="68"/>
@@ -2148,17 +2134,17 @@
       <c r="A12" s="11">
         <v>5</v>
       </c>
-      <c r="B12" s="94" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="95"/>
-      <c r="D12" s="96"/>
+      <c r="B12" s="86" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="87"/>
+      <c r="D12" s="88"/>
       <c r="E12" s="21"/>
       <c r="F12" s="22">
         <v>8</v>
       </c>
       <c r="G12" s="31" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H12" s="23"/>
       <c r="I12" s="68"/>
@@ -2189,17 +2175,17 @@
       <c r="A13" s="11">
         <v>6</v>
       </c>
-      <c r="B13" s="94" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="95"/>
-      <c r="D13" s="96"/>
+      <c r="B13" s="86" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="87"/>
+      <c r="D13" s="88"/>
       <c r="E13" s="21"/>
       <c r="F13" s="22">
         <v>12</v>
       </c>
       <c r="G13" s="31" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H13" s="23"/>
       <c r="I13" s="24"/>
@@ -2230,17 +2216,17 @@
       <c r="A14" s="11">
         <v>7</v>
       </c>
-      <c r="B14" s="94" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" s="95"/>
-      <c r="D14" s="96"/>
+      <c r="B14" s="86" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="87"/>
+      <c r="D14" s="88"/>
       <c r="E14" s="21"/>
       <c r="F14" s="22">
         <v>24</v>
       </c>
       <c r="G14" s="31" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H14" s="23"/>
       <c r="I14" s="24"/>
@@ -2271,17 +2257,17 @@
       <c r="A15" s="11">
         <v>8</v>
       </c>
-      <c r="B15" s="94" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" s="95"/>
-      <c r="D15" s="96"/>
+      <c r="B15" s="86" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="87"/>
+      <c r="D15" s="88"/>
       <c r="E15" s="21"/>
       <c r="F15" s="22">
         <v>40</v>
       </c>
       <c r="G15" s="31" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H15" s="23"/>
       <c r="I15" s="24"/>
@@ -2312,17 +2298,17 @@
       <c r="A16" s="11">
         <v>9</v>
       </c>
-      <c r="B16" s="94" t="s">
-        <v>32</v>
-      </c>
-      <c r="C16" s="95"/>
-      <c r="D16" s="96"/>
+      <c r="B16" s="86" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="87"/>
+      <c r="D16" s="88"/>
       <c r="E16" s="21"/>
       <c r="F16" s="22">
         <v>8</v>
       </c>
       <c r="G16" s="31" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H16" s="23"/>
       <c r="I16" s="24"/>
@@ -2353,17 +2339,17 @@
       <c r="A17" s="11">
         <v>10</v>
       </c>
-      <c r="B17" s="94" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17" s="95"/>
-      <c r="D17" s="96"/>
+      <c r="B17" s="86" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="87"/>
+      <c r="D17" s="88"/>
       <c r="E17" s="21"/>
       <c r="F17" s="22">
         <v>2</v>
       </c>
       <c r="G17" s="31" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H17" s="23"/>
       <c r="I17" s="24"/>
@@ -2394,17 +2380,17 @@
       <c r="A18" s="11">
         <v>11</v>
       </c>
-      <c r="B18" s="94" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" s="95"/>
-      <c r="D18" s="96"/>
+      <c r="B18" s="86" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="87"/>
+      <c r="D18" s="88"/>
       <c r="E18" s="21"/>
       <c r="F18" s="22">
         <v>16</v>
       </c>
       <c r="G18" s="31" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H18" s="23"/>
       <c r="I18" s="24"/>
@@ -2435,17 +2421,17 @@
       <c r="A19" s="11">
         <v>12</v>
       </c>
-      <c r="B19" s="75" t="s">
-        <v>35</v>
-      </c>
-      <c r="C19" s="120"/>
-      <c r="D19" s="121"/>
+      <c r="B19" s="83" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="89"/>
+      <c r="D19" s="90"/>
       <c r="E19" s="21"/>
       <c r="F19" s="22">
         <v>24</v>
       </c>
       <c r="G19" s="31" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H19" s="23"/>
       <c r="I19" s="24"/>
@@ -2476,17 +2462,17 @@
       <c r="A20" s="11">
         <v>13</v>
       </c>
-      <c r="B20" s="75" t="s">
-        <v>36</v>
-      </c>
-      <c r="C20" s="73"/>
-      <c r="D20" s="74"/>
+      <c r="B20" s="83" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="84"/>
+      <c r="D20" s="85"/>
       <c r="E20" s="21"/>
       <c r="F20" s="22">
         <v>40</v>
       </c>
       <c r="G20" s="31" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H20" s="23"/>
       <c r="I20" s="24"/>
@@ -2517,17 +2503,17 @@
       <c r="A21" s="11">
         <v>14</v>
       </c>
-      <c r="B21" s="75" t="s">
-        <v>37</v>
-      </c>
-      <c r="C21" s="76"/>
-      <c r="D21" s="77"/>
+      <c r="B21" s="83" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="114"/>
+      <c r="D21" s="115"/>
       <c r="E21" s="21"/>
       <c r="F21" s="22">
         <v>112</v>
       </c>
       <c r="G21" s="31" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H21" s="23"/>
       <c r="I21" s="24"/>
@@ -2558,17 +2544,17 @@
       <c r="A22" s="11">
         <v>15</v>
       </c>
-      <c r="B22" s="75" t="s">
-        <v>38</v>
-      </c>
-      <c r="C22" s="76"/>
-      <c r="D22" s="77"/>
+      <c r="B22" s="83" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="114"/>
+      <c r="D22" s="115"/>
       <c r="E22" s="21"/>
       <c r="F22" s="57" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G22" s="31" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H22" s="23"/>
       <c r="I22" s="24"/>
@@ -2599,17 +2585,17 @@
       <c r="A23" s="11">
         <v>16</v>
       </c>
-      <c r="B23" s="75" t="s">
-        <v>40</v>
-      </c>
-      <c r="C23" s="76"/>
-      <c r="D23" s="77"/>
+      <c r="B23" s="83" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" s="114"/>
+      <c r="D23" s="115"/>
       <c r="E23" s="21"/>
       <c r="F23" s="22">
         <v>64</v>
       </c>
       <c r="G23" s="31" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H23" s="23"/>
       <c r="I23" s="24"/>
@@ -2638,9 +2624,9 @@
     </row>
     <row r="24" spans="1:31" ht="13.5" thickBot="1">
       <c r="A24" s="11"/>
-      <c r="B24" s="75"/>
-      <c r="C24" s="76"/>
-      <c r="D24" s="77"/>
+      <c r="B24" s="83"/>
+      <c r="C24" s="114"/>
+      <c r="D24" s="115"/>
       <c r="E24" s="21"/>
       <c r="F24" s="22"/>
       <c r="G24" s="32"/>
@@ -2673,17 +2659,17 @@
       <c r="A25" s="11">
         <v>17</v>
       </c>
-      <c r="B25" s="75" t="s">
-        <v>41</v>
-      </c>
-      <c r="C25" s="73"/>
-      <c r="D25" s="74"/>
+      <c r="B25" s="83" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" s="84"/>
+      <c r="D25" s="85"/>
       <c r="E25" s="21"/>
       <c r="F25" s="19">
         <v>10</v>
       </c>
       <c r="G25" s="63" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H25" s="58"/>
       <c r="I25" s="59"/>
@@ -2712,9 +2698,9 @@
     </row>
     <row r="26" spans="1:31" ht="13.5" thickBot="1">
       <c r="A26" s="11"/>
-      <c r="B26" s="72"/>
-      <c r="C26" s="73"/>
-      <c r="D26" s="74"/>
+      <c r="B26" s="113"/>
+      <c r="C26" s="84"/>
+      <c r="D26" s="85"/>
       <c r="E26" s="27"/>
       <c r="F26" s="22"/>
       <c r="G26" s="32"/>
@@ -2747,15 +2733,15 @@
       <c r="A27" s="11">
         <v>18</v>
       </c>
-      <c r="B27" s="75" t="s">
-        <v>42</v>
-      </c>
-      <c r="C27" s="73"/>
-      <c r="D27" s="74"/>
+      <c r="B27" s="83" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27" s="84"/>
+      <c r="D27" s="85"/>
       <c r="E27" s="21"/>
       <c r="F27" s="22"/>
       <c r="G27" s="62" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H27" s="28"/>
       <c r="I27" s="29"/>
@@ -2764,7 +2750,7 @@
       <c r="L27" s="29"/>
       <c r="M27" s="29"/>
       <c r="N27" s="64" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O27" s="29"/>
       <c r="P27" s="29"/>
@@ -2788,15 +2774,15 @@
       <c r="A28" s="11">
         <v>19</v>
       </c>
-      <c r="B28" s="72" t="s">
-        <v>44</v>
-      </c>
-      <c r="C28" s="76"/>
-      <c r="D28" s="77"/>
+      <c r="B28" s="113" t="s">
+        <v>43</v>
+      </c>
+      <c r="C28" s="114"/>
+      <c r="D28" s="115"/>
       <c r="E28" s="21"/>
       <c r="F28" s="22"/>
       <c r="G28" s="62" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H28" s="23"/>
       <c r="I28" s="24"/>
@@ -2808,7 +2794,7 @@
       <c r="O28" s="25"/>
       <c r="P28" s="65"/>
       <c r="Q28" s="66" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="R28" s="24"/>
       <c r="S28" s="24"/>
@@ -2829,15 +2815,15 @@
       <c r="A29" s="11">
         <v>20</v>
       </c>
-      <c r="B29" s="72" t="s">
-        <v>45</v>
-      </c>
-      <c r="C29" s="73"/>
-      <c r="D29" s="74"/>
+      <c r="B29" s="113" t="s">
+        <v>44</v>
+      </c>
+      <c r="C29" s="84"/>
+      <c r="D29" s="85"/>
       <c r="E29" s="21"/>
       <c r="F29" s="22"/>
       <c r="G29" s="62" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H29" s="23"/>
       <c r="I29" s="24"/>
@@ -2855,7 +2841,7 @@
       <c r="U29" s="24"/>
       <c r="V29" s="24"/>
       <c r="W29" s="66" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="X29" s="24"/>
       <c r="Y29" s="24"/>
@@ -2870,15 +2856,15 @@
       <c r="A30" s="11">
         <v>21</v>
       </c>
-      <c r="B30" s="72" t="s">
-        <v>46</v>
-      </c>
-      <c r="C30" s="73"/>
-      <c r="D30" s="74"/>
+      <c r="B30" s="113" t="s">
+        <v>45</v>
+      </c>
+      <c r="C30" s="84"/>
+      <c r="D30" s="85"/>
       <c r="E30" s="21"/>
       <c r="F30" s="22"/>
       <c r="G30" s="62" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H30" s="23"/>
       <c r="I30" s="24"/>
@@ -2899,7 +2885,7 @@
       <c r="X30" s="24"/>
       <c r="Y30" s="24"/>
       <c r="Z30" s="66" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AA30" s="24"/>
       <c r="AB30" s="24"/>
@@ -2911,15 +2897,15 @@
       <c r="A31" s="11">
         <v>22</v>
       </c>
-      <c r="B31" s="72" t="s">
-        <v>48</v>
-      </c>
-      <c r="C31" s="73"/>
-      <c r="D31" s="74"/>
+      <c r="B31" s="113" t="s">
+        <v>47</v>
+      </c>
+      <c r="C31" s="84"/>
+      <c r="D31" s="85"/>
       <c r="E31" s="21"/>
       <c r="F31" s="22"/>
       <c r="G31" s="62" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H31" s="23"/>
       <c r="I31" s="24"/>
@@ -2950,15 +2936,15 @@
       <c r="A32" s="11">
         <v>23</v>
       </c>
-      <c r="B32" s="75" t="s">
-        <v>49</v>
-      </c>
-      <c r="C32" s="73"/>
-      <c r="D32" s="74"/>
+      <c r="B32" s="83" t="s">
+        <v>48</v>
+      </c>
+      <c r="C32" s="84"/>
+      <c r="D32" s="85"/>
       <c r="E32" s="21"/>
       <c r="F32" s="22"/>
       <c r="G32" s="62" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H32" s="23"/>
       <c r="I32" s="24"/>
@@ -2989,9 +2975,9 @@
       <c r="A33" s="11">
         <v>24</v>
       </c>
-      <c r="B33" s="108"/>
-      <c r="C33" s="109"/>
-      <c r="D33" s="110"/>
+      <c r="B33" s="110"/>
+      <c r="C33" s="111"/>
+      <c r="D33" s="112"/>
       <c r="E33" s="21"/>
       <c r="F33" s="41"/>
       <c r="G33" s="43"/>
@@ -3022,11 +3008,11 @@
     </row>
     <row r="34" spans="1:31" ht="13.5" thickBot="1">
       <c r="A34" s="7"/>
-      <c r="B34" s="97" t="s">
-        <v>50</v>
-      </c>
-      <c r="C34" s="97"/>
-      <c r="D34" s="98"/>
+      <c r="B34" s="95" t="s">
+        <v>49</v>
+      </c>
+      <c r="C34" s="95"/>
+      <c r="D34" s="96"/>
       <c r="E34" s="48"/>
       <c r="F34" s="49">
         <f>SUM(F8:F33)</f>
@@ -3060,6 +3046,36 @@
     </row>
   </sheetData>
   <mergeCells count="46">
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I3:O3"/>
+    <mergeCell ref="I4:O4"/>
+    <mergeCell ref="I5:O5"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="B30:D30"/>
     <mergeCell ref="A1:AE1"/>
     <mergeCell ref="D2:AE2"/>
     <mergeCell ref="H6:AE6"/>
@@ -3074,38 +3090,8 @@
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B31:D31"/>
     <mergeCell ref="P3:T3"/>
     <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I3:O3"/>
-    <mergeCell ref="I4:O4"/>
-    <mergeCell ref="I5:O5"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B23:D23"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="0.98425196850393704" bottom="0.78740157480314965" header="0.51181102362204722" footer="0.51181102362204722"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3119,8 +3105,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AE34"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0" xr3:uid="{958C4451-9541-5A59-BF78-D2F731DF1C81}">
-      <selection activeCell="D2" sqref="D2:AE2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0" xr3:uid="{958C4451-9541-5A59-BF78-D2F731DF1C81}">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -3137,107 +3123,110 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" s="15" customFormat="1" ht="18">
-      <c r="A1" s="122" t="s">
-        <v>51</v>
-      </c>
-      <c r="B1" s="123"/>
-      <c r="C1" s="123"/>
-      <c r="D1" s="123"/>
-      <c r="E1" s="123"/>
-      <c r="F1" s="123"/>
-      <c r="G1" s="123"/>
-      <c r="H1" s="123"/>
-      <c r="I1" s="123"/>
-      <c r="J1" s="123"/>
-      <c r="K1" s="123"/>
-      <c r="L1" s="123"/>
-      <c r="M1" s="123"/>
-      <c r="N1" s="123"/>
-      <c r="O1" s="123"/>
-      <c r="P1" s="123"/>
-      <c r="Q1" s="123"/>
-      <c r="R1" s="123"/>
-      <c r="S1" s="123"/>
-      <c r="T1" s="123"/>
-      <c r="U1" s="123"/>
-      <c r="V1" s="123"/>
-      <c r="W1" s="123"/>
-      <c r="X1" s="123"/>
-      <c r="Y1" s="123"/>
-      <c r="Z1" s="123"/>
-      <c r="AA1" s="123"/>
-      <c r="AB1" s="123"/>
-      <c r="AC1" s="123"/>
-      <c r="AD1" s="123"/>
-      <c r="AE1" s="124"/>
+      <c r="A1" s="130" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="131"/>
+      <c r="C1" s="131"/>
+      <c r="D1" s="131"/>
+      <c r="E1" s="131"/>
+      <c r="F1" s="131"/>
+      <c r="G1" s="131"/>
+      <c r="H1" s="131"/>
+      <c r="I1" s="131"/>
+      <c r="J1" s="131"/>
+      <c r="K1" s="131"/>
+      <c r="L1" s="131"/>
+      <c r="M1" s="131"/>
+      <c r="N1" s="131"/>
+      <c r="O1" s="131"/>
+      <c r="P1" s="131"/>
+      <c r="Q1" s="131"/>
+      <c r="R1" s="131"/>
+      <c r="S1" s="131"/>
+      <c r="T1" s="131"/>
+      <c r="U1" s="131"/>
+      <c r="V1" s="131"/>
+      <c r="W1" s="131"/>
+      <c r="X1" s="131"/>
+      <c r="Y1" s="131"/>
+      <c r="Z1" s="131"/>
+      <c r="AA1" s="131"/>
+      <c r="AB1" s="131"/>
+      <c r="AC1" s="131"/>
+      <c r="AD1" s="131"/>
+      <c r="AE1" s="132"/>
     </row>
     <row r="2" spans="1:31" s="15" customFormat="1" ht="18.75" thickBot="1">
-      <c r="A2" s="128" t="s">
+      <c r="A2" s="136" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="129"/>
+      <c r="B2" s="137"/>
       <c r="C2" s="55"/>
-      <c r="D2" s="125" t="str">
+      <c r="D2" s="133" t="str">
         <f>Basplan!D2</f>
         <v>Deepoid AB CDIO</v>
       </c>
-      <c r="E2" s="125"/>
-      <c r="F2" s="125"/>
-      <c r="G2" s="126"/>
-      <c r="H2" s="126"/>
-      <c r="I2" s="126"/>
-      <c r="J2" s="126"/>
-      <c r="K2" s="126"/>
-      <c r="L2" s="126"/>
-      <c r="M2" s="126"/>
-      <c r="N2" s="126"/>
-      <c r="O2" s="126"/>
-      <c r="P2" s="126"/>
-      <c r="Q2" s="126"/>
-      <c r="R2" s="126"/>
-      <c r="S2" s="126"/>
-      <c r="T2" s="126"/>
-      <c r="U2" s="126"/>
-      <c r="V2" s="126"/>
-      <c r="W2" s="126"/>
-      <c r="X2" s="126"/>
-      <c r="Y2" s="126"/>
-      <c r="Z2" s="126"/>
-      <c r="AA2" s="126"/>
-      <c r="AB2" s="126"/>
-      <c r="AC2" s="126"/>
-      <c r="AD2" s="126"/>
-      <c r="AE2" s="127"/>
+      <c r="E2" s="133"/>
+      <c r="F2" s="133"/>
+      <c r="G2" s="134"/>
+      <c r="H2" s="134"/>
+      <c r="I2" s="134"/>
+      <c r="J2" s="134"/>
+      <c r="K2" s="134"/>
+      <c r="L2" s="134"/>
+      <c r="M2" s="134"/>
+      <c r="N2" s="134"/>
+      <c r="O2" s="134"/>
+      <c r="P2" s="134"/>
+      <c r="Q2" s="134"/>
+      <c r="R2" s="134"/>
+      <c r="S2" s="134"/>
+      <c r="T2" s="134"/>
+      <c r="U2" s="134"/>
+      <c r="V2" s="134"/>
+      <c r="W2" s="134"/>
+      <c r="X2" s="134"/>
+      <c r="Y2" s="134"/>
+      <c r="Z2" s="134"/>
+      <c r="AA2" s="134"/>
+      <c r="AB2" s="134"/>
+      <c r="AC2" s="134"/>
+      <c r="AD2" s="134"/>
+      <c r="AE2" s="135"/>
     </row>
     <row r="3" spans="1:31" ht="15.75">
-      <c r="A3" s="78" t="s">
+      <c r="A3" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="79"/>
+      <c r="B3" s="92"/>
       <c r="C3" s="56"/>
-      <c r="D3" s="130" t="str">
+      <c r="D3" s="138" t="str">
         <f>Basplan!D3</f>
         <v>Grupp 6</v>
       </c>
-      <c r="E3" s="130"/>
-      <c r="F3" s="131"/>
-      <c r="G3" s="79" t="s">
+      <c r="E3" s="138"/>
+      <c r="F3" s="139"/>
+      <c r="G3" s="92" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="79"/>
-      <c r="I3" s="88"/>
-      <c r="J3" s="88"/>
-      <c r="K3" s="88"/>
-      <c r="L3" s="88"/>
-      <c r="M3" s="88"/>
-      <c r="N3" s="88"/>
-      <c r="O3" s="89"/>
-      <c r="P3" s="78" t="s">
+      <c r="H3" s="92"/>
+      <c r="I3" s="116">
+        <f ca="1">NOW()</f>
+        <v>43366.704446064818</v>
+      </c>
+      <c r="J3" s="116"/>
+      <c r="K3" s="116"/>
+      <c r="L3" s="116"/>
+      <c r="M3" s="116"/>
+      <c r="N3" s="116"/>
+      <c r="O3" s="117"/>
+      <c r="P3" s="91" t="s">
         <v>6</v>
       </c>
-      <c r="Q3" s="79"/>
-      <c r="R3" s="79"/>
-      <c r="S3" s="79"/>
+      <c r="Q3" s="92"/>
+      <c r="R3" s="92"/>
+      <c r="S3" s="92"/>
       <c r="T3" s="5"/>
       <c r="U3" s="5"/>
       <c r="V3" s="5"/>
@@ -3252,28 +3241,30 @@
       <c r="AE3" s="4"/>
     </row>
     <row r="4" spans="1:31" ht="15.75">
-      <c r="A4" s="84" t="s">
+      <c r="A4" s="105" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="85"/>
+      <c r="B4" s="106"/>
       <c r="C4" s="13"/>
-      <c r="D4" s="90" t="str">
+      <c r="D4" s="118" t="str">
         <f>Basplan!D4</f>
         <v>Deepoid AB</v>
       </c>
-      <c r="E4" s="90"/>
-      <c r="F4" s="91"/>
-      <c r="G4" s="85" t="s">
+      <c r="E4" s="118"/>
+      <c r="F4" s="119"/>
+      <c r="G4" s="106" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="85"/>
-      <c r="I4" s="90"/>
-      <c r="J4" s="90"/>
-      <c r="K4" s="90"/>
-      <c r="L4" s="90"/>
-      <c r="M4" s="90"/>
-      <c r="N4" s="90"/>
-      <c r="O4" s="91"/>
+      <c r="H4" s="106"/>
+      <c r="I4" s="118">
+        <v>1</v>
+      </c>
+      <c r="J4" s="118"/>
+      <c r="K4" s="118"/>
+      <c r="L4" s="118"/>
+      <c r="M4" s="118"/>
+      <c r="N4" s="118"/>
+      <c r="O4" s="119"/>
       <c r="P4" s="3"/>
       <c r="Q4" s="14"/>
       <c r="R4" s="14"/>
@@ -3292,28 +3283,30 @@
       <c r="AE4" s="4"/>
     </row>
     <row r="5" spans="1:31" ht="16.5" thickBot="1">
-      <c r="A5" s="86" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="87"/>
+      <c r="A5" s="103" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="104"/>
       <c r="C5" s="6"/>
-      <c r="D5" s="92" t="str">
+      <c r="D5" s="120" t="str">
         <f>Basplan!D5</f>
         <v>CDIO</v>
       </c>
-      <c r="E5" s="92"/>
-      <c r="F5" s="93"/>
-      <c r="G5" s="87" t="s">
+      <c r="E5" s="120"/>
+      <c r="F5" s="121"/>
+      <c r="G5" s="104" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="104"/>
+      <c r="I5" s="120" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="87"/>
-      <c r="I5" s="92"/>
-      <c r="J5" s="92"/>
-      <c r="K5" s="92"/>
-      <c r="L5" s="92"/>
-      <c r="M5" s="92"/>
-      <c r="N5" s="92"/>
-      <c r="O5" s="93"/>
+      <c r="J5" s="120"/>
+      <c r="K5" s="120"/>
+      <c r="L5" s="120"/>
+      <c r="M5" s="120"/>
+      <c r="N5" s="120"/>
+      <c r="O5" s="121"/>
       <c r="P5" s="3"/>
       <c r="Q5" s="5"/>
       <c r="R5" s="5"/>
@@ -3332,52 +3325,52 @@
       <c r="AE5" s="4"/>
     </row>
     <row r="6" spans="1:31" s="2" customFormat="1" ht="16.5" thickBot="1">
-      <c r="A6" s="132" t="s">
+      <c r="A6" s="140" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="141"/>
+      <c r="C6" s="141"/>
+      <c r="D6" s="141"/>
+      <c r="E6" s="141"/>
+      <c r="F6" s="141"/>
+      <c r="G6" s="142"/>
+      <c r="H6" s="77" t="s">
         <v>52</v>
       </c>
-      <c r="B6" s="133"/>
-      <c r="C6" s="133"/>
-      <c r="D6" s="133"/>
-      <c r="E6" s="133"/>
-      <c r="F6" s="133"/>
-      <c r="G6" s="134"/>
-      <c r="H6" s="82" t="s">
-        <v>53</v>
-      </c>
-      <c r="I6" s="83"/>
-      <c r="J6" s="83"/>
-      <c r="K6" s="83"/>
-      <c r="L6" s="83"/>
-      <c r="M6" s="83"/>
-      <c r="N6" s="83"/>
-      <c r="O6" s="83"/>
-      <c r="P6" s="83"/>
-      <c r="Q6" s="83"/>
-      <c r="R6" s="83"/>
-      <c r="S6" s="83"/>
-      <c r="T6" s="83"/>
-      <c r="U6" s="83"/>
-      <c r="V6" s="83"/>
-      <c r="W6" s="83"/>
-      <c r="X6" s="83"/>
-      <c r="Y6" s="83"/>
-      <c r="Z6" s="83"/>
-      <c r="AA6" s="83"/>
-      <c r="AB6" s="83"/>
-      <c r="AC6" s="83"/>
-      <c r="AD6" s="83"/>
-      <c r="AE6" s="116"/>
+      <c r="I6" s="78"/>
+      <c r="J6" s="78"/>
+      <c r="K6" s="78"/>
+      <c r="L6" s="78"/>
+      <c r="M6" s="78"/>
+      <c r="N6" s="78"/>
+      <c r="O6" s="78"/>
+      <c r="P6" s="78"/>
+      <c r="Q6" s="78"/>
+      <c r="R6" s="78"/>
+      <c r="S6" s="78"/>
+      <c r="T6" s="78"/>
+      <c r="U6" s="78"/>
+      <c r="V6" s="78"/>
+      <c r="W6" s="78"/>
+      <c r="X6" s="78"/>
+      <c r="Y6" s="78"/>
+      <c r="Z6" s="78"/>
+      <c r="AA6" s="78"/>
+      <c r="AB6" s="78"/>
+      <c r="AC6" s="78"/>
+      <c r="AD6" s="78"/>
+      <c r="AE6" s="79"/>
     </row>
     <row r="7" spans="1:31" ht="13.5" thickBot="1">
       <c r="A7" s="7"/>
-      <c r="B7" s="117" t="s">
-        <v>54</v>
-      </c>
-      <c r="C7" s="118"/>
-      <c r="D7" s="118"/>
-      <c r="E7" s="118"/>
-      <c r="F7" s="118"/>
-      <c r="G7" s="119"/>
+      <c r="B7" s="80" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="81"/>
+      <c r="D7" s="81"/>
+      <c r="E7" s="81"/>
+      <c r="F7" s="81"/>
+      <c r="G7" s="82"/>
       <c r="H7" s="35">
         <f>Basplan!H7</f>
         <v>36</v>
@@ -3471,28 +3464,30 @@
         <v>6</v>
       </c>
       <c r="AE7" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:31">
       <c r="A8" s="12"/>
-      <c r="B8" s="140" t="s">
-        <v>56</v>
-      </c>
-      <c r="C8" s="141"/>
-      <c r="D8" s="141"/>
-      <c r="E8" s="141"/>
-      <c r="F8" s="141"/>
-      <c r="G8" s="142"/>
+      <c r="B8" s="122" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="123"/>
+      <c r="D8" s="123"/>
+      <c r="E8" s="123"/>
+      <c r="F8" s="123"/>
+      <c r="G8" s="124"/>
       <c r="H8" s="30">
-        <v>5</v>
-      </c>
-      <c r="I8" s="20"/>
-      <c r="J8" s="20"/>
+        <v>12</v>
+      </c>
+      <c r="I8" s="20">
+        <v>9</v>
+      </c>
+      <c r="J8" s="20">
+        <v>14</v>
+      </c>
       <c r="K8" s="20"/>
-      <c r="L8" s="20">
-        <v>4</v>
-      </c>
+      <c r="L8" s="20"/>
       <c r="M8" s="20"/>
       <c r="N8" s="20"/>
       <c r="O8" s="20"/>
@@ -3513,35 +3508,33 @@
       <c r="AD8" s="36"/>
       <c r="AE8" s="33">
         <f t="shared" ref="AE8:AE33" si="0">SUM(H8:AD8)</f>
-        <v>9</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:31">
       <c r="A9" s="12"/>
-      <c r="B9" s="72" t="s">
-        <v>57</v>
-      </c>
-      <c r="C9" s="73"/>
-      <c r="D9" s="73"/>
-      <c r="E9" s="73"/>
-      <c r="F9" s="73"/>
-      <c r="G9" s="74"/>
-      <c r="H9" s="23"/>
+      <c r="B9" s="113" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="84"/>
+      <c r="D9" s="84"/>
+      <c r="E9" s="84"/>
+      <c r="F9" s="84"/>
+      <c r="G9" s="85"/>
+      <c r="H9" s="23">
+        <v>10</v>
+      </c>
       <c r="I9" s="24">
-        <v>44</v>
-      </c>
-      <c r="J9" s="24"/>
-      <c r="K9" s="24">
-        <v>3</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="J9" s="24">
+        <v>16</v>
+      </c>
+      <c r="K9" s="24"/>
       <c r="L9" s="24"/>
-      <c r="M9" s="24">
-        <v>4</v>
-      </c>
+      <c r="M9" s="24"/>
       <c r="N9" s="24"/>
-      <c r="O9" s="24">
-        <v>3</v>
-      </c>
+      <c r="O9" s="24"/>
       <c r="P9" s="24"/>
       <c r="Q9" s="24"/>
       <c r="R9" s="24"/>
@@ -3559,30 +3552,24 @@
       <c r="AD9" s="37"/>
       <c r="AE9" s="34">
         <f t="shared" si="0"/>
-        <v>54</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:31">
       <c r="A10" s="12"/>
-      <c r="B10" s="72" t="s">
-        <v>58</v>
-      </c>
-      <c r="C10" s="73"/>
-      <c r="D10" s="73"/>
-      <c r="E10" s="73"/>
-      <c r="F10" s="73"/>
-      <c r="G10" s="74"/>
-      <c r="H10" s="23">
-        <v>5</v>
-      </c>
+      <c r="B10" s="113"/>
+      <c r="C10" s="84"/>
+      <c r="D10" s="84"/>
+      <c r="E10" s="84"/>
+      <c r="F10" s="84"/>
+      <c r="G10" s="85"/>
+      <c r="H10" s="23"/>
       <c r="I10" s="24"/>
       <c r="J10" s="24"/>
       <c r="K10" s="24"/>
       <c r="L10" s="24"/>
       <c r="M10" s="24"/>
-      <c r="N10" s="24">
-        <v>5</v>
-      </c>
+      <c r="N10" s="24"/>
       <c r="O10" s="24"/>
       <c r="P10" s="24"/>
       <c r="Q10" s="24"/>
@@ -3601,31 +3588,23 @@
       <c r="AD10" s="37"/>
       <c r="AE10" s="34">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:31">
       <c r="A11" s="12"/>
-      <c r="B11" s="72" t="s">
-        <v>59</v>
-      </c>
-      <c r="C11" s="73"/>
-      <c r="D11" s="73"/>
-      <c r="E11" s="73"/>
-      <c r="F11" s="73"/>
-      <c r="G11" s="74"/>
+      <c r="B11" s="113"/>
+      <c r="C11" s="84"/>
+      <c r="D11" s="84"/>
+      <c r="E11" s="84"/>
+      <c r="F11" s="84"/>
+      <c r="G11" s="85"/>
       <c r="H11" s="23"/>
       <c r="I11" s="24"/>
-      <c r="J11" s="24">
-        <v>5</v>
-      </c>
+      <c r="J11" s="24"/>
       <c r="K11" s="24"/>
-      <c r="L11" s="24">
-        <v>5</v>
-      </c>
-      <c r="M11" s="24">
-        <v>3</v>
-      </c>
+      <c r="L11" s="24"/>
+      <c r="M11" s="24"/>
       <c r="N11" s="24"/>
       <c r="O11" s="24"/>
       <c r="P11" s="24"/>
@@ -3645,35 +3624,25 @@
       <c r="AD11" s="37"/>
       <c r="AE11" s="34">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:31">
       <c r="A12" s="12"/>
-      <c r="B12" s="72" t="s">
-        <v>60</v>
-      </c>
-      <c r="C12" s="73"/>
-      <c r="D12" s="73"/>
-      <c r="E12" s="73"/>
-      <c r="F12" s="73"/>
-      <c r="G12" s="74"/>
-      <c r="H12" s="23">
-        <v>8</v>
-      </c>
+      <c r="B12" s="113"/>
+      <c r="C12" s="84"/>
+      <c r="D12" s="84"/>
+      <c r="E12" s="84"/>
+      <c r="F12" s="84"/>
+      <c r="G12" s="85"/>
+      <c r="H12" s="23"/>
       <c r="I12" s="24"/>
       <c r="J12" s="24"/>
-      <c r="K12" s="24">
-        <v>4</v>
-      </c>
+      <c r="K12" s="24"/>
       <c r="L12" s="24"/>
-      <c r="M12" s="24">
-        <v>6</v>
-      </c>
+      <c r="M12" s="24"/>
       <c r="N12" s="24"/>
-      <c r="O12" s="24">
-        <v>6</v>
-      </c>
+      <c r="O12" s="24"/>
       <c r="P12" s="24"/>
       <c r="Q12" s="24"/>
       <c r="R12" s="24"/>
@@ -3691,17 +3660,17 @@
       <c r="AD12" s="37"/>
       <c r="AE12" s="34">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:31">
       <c r="A13" s="12"/>
-      <c r="B13" s="72"/>
-      <c r="C13" s="73"/>
-      <c r="D13" s="73"/>
-      <c r="E13" s="73"/>
-      <c r="F13" s="73"/>
-      <c r="G13" s="74"/>
+      <c r="B13" s="113"/>
+      <c r="C13" s="84"/>
+      <c r="D13" s="84"/>
+      <c r="E13" s="84"/>
+      <c r="F13" s="84"/>
+      <c r="G13" s="85"/>
       <c r="H13" s="23"/>
       <c r="I13" s="24"/>
       <c r="J13" s="24"/>
@@ -3732,12 +3701,12 @@
     </row>
     <row r="14" spans="1:31">
       <c r="A14" s="12"/>
-      <c r="B14" s="72"/>
-      <c r="C14" s="73"/>
-      <c r="D14" s="73"/>
-      <c r="E14" s="73"/>
-      <c r="F14" s="73"/>
-      <c r="G14" s="74"/>
+      <c r="B14" s="113"/>
+      <c r="C14" s="84"/>
+      <c r="D14" s="84"/>
+      <c r="E14" s="84"/>
+      <c r="F14" s="84"/>
+      <c r="G14" s="85"/>
       <c r="H14" s="23"/>
       <c r="I14" s="24"/>
       <c r="J14" s="24"/>
@@ -3768,12 +3737,12 @@
     </row>
     <row r="15" spans="1:31">
       <c r="A15" s="12"/>
-      <c r="B15" s="72"/>
-      <c r="C15" s="73"/>
-      <c r="D15" s="73"/>
-      <c r="E15" s="73"/>
-      <c r="F15" s="73"/>
-      <c r="G15" s="74"/>
+      <c r="B15" s="113"/>
+      <c r="C15" s="84"/>
+      <c r="D15" s="84"/>
+      <c r="E15" s="84"/>
+      <c r="F15" s="84"/>
+      <c r="G15" s="85"/>
       <c r="H15" s="23"/>
       <c r="I15" s="24"/>
       <c r="J15" s="24"/>
@@ -3804,12 +3773,12 @@
     </row>
     <row r="16" spans="1:31">
       <c r="A16" s="12"/>
-      <c r="B16" s="72"/>
-      <c r="C16" s="73"/>
-      <c r="D16" s="73"/>
-      <c r="E16" s="73"/>
-      <c r="F16" s="73"/>
-      <c r="G16" s="74"/>
+      <c r="B16" s="113"/>
+      <c r="C16" s="84"/>
+      <c r="D16" s="84"/>
+      <c r="E16" s="84"/>
+      <c r="F16" s="84"/>
+      <c r="G16" s="85"/>
       <c r="H16" s="23"/>
       <c r="I16" s="24"/>
       <c r="J16" s="24"/>
@@ -3840,12 +3809,12 @@
     </row>
     <row r="17" spans="1:31">
       <c r="A17" s="12"/>
-      <c r="B17" s="72"/>
-      <c r="C17" s="73"/>
-      <c r="D17" s="73"/>
-      <c r="E17" s="73"/>
-      <c r="F17" s="73"/>
-      <c r="G17" s="74"/>
+      <c r="B17" s="113"/>
+      <c r="C17" s="84"/>
+      <c r="D17" s="84"/>
+      <c r="E17" s="84"/>
+      <c r="F17" s="84"/>
+      <c r="G17" s="85"/>
       <c r="H17" s="23"/>
       <c r="I17" s="24"/>
       <c r="J17" s="24"/>
@@ -3876,12 +3845,12 @@
     </row>
     <row r="18" spans="1:31">
       <c r="A18" s="12"/>
-      <c r="B18" s="72"/>
-      <c r="C18" s="73"/>
-      <c r="D18" s="73"/>
-      <c r="E18" s="73"/>
-      <c r="F18" s="73"/>
-      <c r="G18" s="74"/>
+      <c r="B18" s="113"/>
+      <c r="C18" s="84"/>
+      <c r="D18" s="84"/>
+      <c r="E18" s="84"/>
+      <c r="F18" s="84"/>
+      <c r="G18" s="85"/>
       <c r="H18" s="23"/>
       <c r="I18" s="24"/>
       <c r="J18" s="24"/>
@@ -3912,12 +3881,12 @@
     </row>
     <row r="19" spans="1:31">
       <c r="A19" s="12"/>
-      <c r="B19" s="72"/>
-      <c r="C19" s="73"/>
-      <c r="D19" s="73"/>
-      <c r="E19" s="73"/>
-      <c r="F19" s="73"/>
-      <c r="G19" s="74"/>
+      <c r="B19" s="113"/>
+      <c r="C19" s="84"/>
+      <c r="D19" s="84"/>
+      <c r="E19" s="84"/>
+      <c r="F19" s="84"/>
+      <c r="G19" s="85"/>
       <c r="H19" s="23"/>
       <c r="I19" s="24"/>
       <c r="J19" s="24"/>
@@ -3948,12 +3917,12 @@
     </row>
     <row r="20" spans="1:31">
       <c r="A20" s="12"/>
-      <c r="B20" s="72"/>
-      <c r="C20" s="73"/>
-      <c r="D20" s="73"/>
-      <c r="E20" s="73"/>
-      <c r="F20" s="73"/>
-      <c r="G20" s="74"/>
+      <c r="B20" s="113"/>
+      <c r="C20" s="84"/>
+      <c r="D20" s="84"/>
+      <c r="E20" s="84"/>
+      <c r="F20" s="84"/>
+      <c r="G20" s="85"/>
       <c r="H20" s="23"/>
       <c r="I20" s="24"/>
       <c r="J20" s="24"/>
@@ -3984,12 +3953,12 @@
     </row>
     <row r="21" spans="1:31">
       <c r="A21" s="12"/>
-      <c r="B21" s="72"/>
-      <c r="C21" s="73"/>
-      <c r="D21" s="73"/>
-      <c r="E21" s="73"/>
-      <c r="F21" s="73"/>
-      <c r="G21" s="74"/>
+      <c r="B21" s="113"/>
+      <c r="C21" s="84"/>
+      <c r="D21" s="84"/>
+      <c r="E21" s="84"/>
+      <c r="F21" s="84"/>
+      <c r="G21" s="85"/>
       <c r="H21" s="23"/>
       <c r="I21" s="24"/>
       <c r="J21" s="24"/>
@@ -4020,12 +3989,12 @@
     </row>
     <row r="22" spans="1:31">
       <c r="A22" s="12"/>
-      <c r="B22" s="72"/>
-      <c r="C22" s="73"/>
-      <c r="D22" s="73"/>
-      <c r="E22" s="73"/>
-      <c r="F22" s="73"/>
-      <c r="G22" s="74"/>
+      <c r="B22" s="113"/>
+      <c r="C22" s="84"/>
+      <c r="D22" s="84"/>
+      <c r="E22" s="84"/>
+      <c r="F22" s="84"/>
+      <c r="G22" s="85"/>
       <c r="H22" s="23"/>
       <c r="I22" s="24"/>
       <c r="J22" s="24"/>
@@ -4056,12 +4025,12 @@
     </row>
     <row r="23" spans="1:31">
       <c r="A23" s="12"/>
-      <c r="B23" s="72"/>
-      <c r="C23" s="73"/>
-      <c r="D23" s="73"/>
-      <c r="E23" s="73"/>
-      <c r="F23" s="73"/>
-      <c r="G23" s="74"/>
+      <c r="B23" s="113"/>
+      <c r="C23" s="84"/>
+      <c r="D23" s="84"/>
+      <c r="E23" s="84"/>
+      <c r="F23" s="84"/>
+      <c r="G23" s="85"/>
       <c r="H23" s="23"/>
       <c r="I23" s="24"/>
       <c r="J23" s="24"/>
@@ -4092,12 +4061,12 @@
     </row>
     <row r="24" spans="1:31">
       <c r="A24" s="12"/>
-      <c r="B24" s="72"/>
-      <c r="C24" s="73"/>
-      <c r="D24" s="73"/>
-      <c r="E24" s="73"/>
-      <c r="F24" s="73"/>
-      <c r="G24" s="74"/>
+      <c r="B24" s="113"/>
+      <c r="C24" s="84"/>
+      <c r="D24" s="84"/>
+      <c r="E24" s="84"/>
+      <c r="F24" s="84"/>
+      <c r="G24" s="85"/>
       <c r="H24" s="23"/>
       <c r="I24" s="24"/>
       <c r="J24" s="24"/>
@@ -4128,12 +4097,12 @@
     </row>
     <row r="25" spans="1:31">
       <c r="A25" s="12"/>
-      <c r="B25" s="72"/>
-      <c r="C25" s="73"/>
-      <c r="D25" s="73"/>
-      <c r="E25" s="73"/>
-      <c r="F25" s="73"/>
-      <c r="G25" s="74"/>
+      <c r="B25" s="113"/>
+      <c r="C25" s="84"/>
+      <c r="D25" s="84"/>
+      <c r="E25" s="84"/>
+      <c r="F25" s="84"/>
+      <c r="G25" s="85"/>
       <c r="H25" s="23"/>
       <c r="I25" s="24"/>
       <c r="J25" s="24"/>
@@ -4164,12 +4133,12 @@
     </row>
     <row r="26" spans="1:31">
       <c r="A26" s="12"/>
-      <c r="B26" s="72"/>
-      <c r="C26" s="73"/>
-      <c r="D26" s="73"/>
-      <c r="E26" s="73"/>
-      <c r="F26" s="73"/>
-      <c r="G26" s="74"/>
+      <c r="B26" s="113"/>
+      <c r="C26" s="84"/>
+      <c r="D26" s="84"/>
+      <c r="E26" s="84"/>
+      <c r="F26" s="84"/>
+      <c r="G26" s="85"/>
       <c r="H26" s="23"/>
       <c r="I26" s="24"/>
       <c r="J26" s="24"/>
@@ -4200,12 +4169,12 @@
     </row>
     <row r="27" spans="1:31">
       <c r="A27" s="12"/>
-      <c r="B27" s="72"/>
-      <c r="C27" s="73"/>
-      <c r="D27" s="73"/>
-      <c r="E27" s="73"/>
-      <c r="F27" s="73"/>
-      <c r="G27" s="74"/>
+      <c r="B27" s="113"/>
+      <c r="C27" s="84"/>
+      <c r="D27" s="84"/>
+      <c r="E27" s="84"/>
+      <c r="F27" s="84"/>
+      <c r="G27" s="85"/>
       <c r="H27" s="23"/>
       <c r="I27" s="24"/>
       <c r="J27" s="24"/>
@@ -4236,12 +4205,12 @@
     </row>
     <row r="28" spans="1:31">
       <c r="A28" s="42"/>
-      <c r="B28" s="72"/>
-      <c r="C28" s="73"/>
-      <c r="D28" s="73"/>
-      <c r="E28" s="73"/>
-      <c r="F28" s="73"/>
-      <c r="G28" s="74"/>
+      <c r="B28" s="113"/>
+      <c r="C28" s="84"/>
+      <c r="D28" s="84"/>
+      <c r="E28" s="84"/>
+      <c r="F28" s="84"/>
+      <c r="G28" s="85"/>
       <c r="H28" s="23"/>
       <c r="I28" s="24"/>
       <c r="J28" s="24"/>
@@ -4272,12 +4241,12 @@
     </row>
     <row r="29" spans="1:31">
       <c r="A29" s="42"/>
-      <c r="B29" s="72"/>
-      <c r="C29" s="73"/>
-      <c r="D29" s="73"/>
-      <c r="E29" s="73"/>
-      <c r="F29" s="73"/>
-      <c r="G29" s="74"/>
+      <c r="B29" s="113"/>
+      <c r="C29" s="84"/>
+      <c r="D29" s="84"/>
+      <c r="E29" s="84"/>
+      <c r="F29" s="84"/>
+      <c r="G29" s="85"/>
       <c r="H29" s="23"/>
       <c r="I29" s="24"/>
       <c r="J29" s="24"/>
@@ -4308,12 +4277,12 @@
     </row>
     <row r="30" spans="1:31">
       <c r="A30" s="12"/>
-      <c r="B30" s="72"/>
-      <c r="C30" s="73"/>
-      <c r="D30" s="73"/>
-      <c r="E30" s="73"/>
-      <c r="F30" s="73"/>
-      <c r="G30" s="74"/>
+      <c r="B30" s="113"/>
+      <c r="C30" s="84"/>
+      <c r="D30" s="84"/>
+      <c r="E30" s="84"/>
+      <c r="F30" s="84"/>
+      <c r="G30" s="85"/>
       <c r="H30" s="23"/>
       <c r="I30" s="24"/>
       <c r="J30" s="24"/>
@@ -4344,12 +4313,12 @@
     </row>
     <row r="31" spans="1:31">
       <c r="A31" s="12"/>
-      <c r="B31" s="72"/>
-      <c r="C31" s="73"/>
-      <c r="D31" s="73"/>
-      <c r="E31" s="73"/>
-      <c r="F31" s="73"/>
-      <c r="G31" s="74"/>
+      <c r="B31" s="113"/>
+      <c r="C31" s="84"/>
+      <c r="D31" s="84"/>
+      <c r="E31" s="84"/>
+      <c r="F31" s="84"/>
+      <c r="G31" s="85"/>
       <c r="H31" s="23"/>
       <c r="I31" s="24"/>
       <c r="J31" s="24"/>
@@ -4380,12 +4349,12 @@
     </row>
     <row r="32" spans="1:31">
       <c r="A32" s="12"/>
-      <c r="B32" s="72"/>
-      <c r="C32" s="73"/>
-      <c r="D32" s="73"/>
-      <c r="E32" s="73"/>
-      <c r="F32" s="73"/>
-      <c r="G32" s="74"/>
+      <c r="B32" s="113"/>
+      <c r="C32" s="84"/>
+      <c r="D32" s="84"/>
+      <c r="E32" s="84"/>
+      <c r="F32" s="84"/>
+      <c r="G32" s="85"/>
       <c r="H32" s="23"/>
       <c r="I32" s="24"/>
       <c r="J32" s="24"/>
@@ -4416,12 +4385,12 @@
     </row>
     <row r="33" spans="1:31" ht="13.5" thickBot="1">
       <c r="A33" s="12"/>
-      <c r="B33" s="135"/>
-      <c r="C33" s="136"/>
-      <c r="D33" s="136"/>
-      <c r="E33" s="136"/>
-      <c r="F33" s="136"/>
-      <c r="G33" s="137"/>
+      <c r="B33" s="125"/>
+      <c r="C33" s="126"/>
+      <c r="D33" s="126"/>
+      <c r="E33" s="126"/>
+      <c r="F33" s="126"/>
+      <c r="G33" s="127"/>
       <c r="H33" s="38"/>
       <c r="I33" s="26"/>
       <c r="J33" s="26"/>
@@ -4452,45 +4421,45 @@
     </row>
     <row r="34" spans="1:31" ht="13.5" thickBot="1">
       <c r="A34" s="9"/>
-      <c r="B34" s="138" t="s">
-        <v>61</v>
-      </c>
-      <c r="C34" s="138"/>
-      <c r="D34" s="138"/>
-      <c r="E34" s="138"/>
-      <c r="F34" s="138"/>
-      <c r="G34" s="139"/>
+      <c r="B34" s="128" t="s">
+        <v>56</v>
+      </c>
+      <c r="C34" s="128"/>
+      <c r="D34" s="128"/>
+      <c r="E34" s="128"/>
+      <c r="F34" s="128"/>
+      <c r="G34" s="129"/>
       <c r="H34" s="40">
         <f>SUM(H8:H33)</f>
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="I34" s="46">
         <f>SUM(I8:I33)</f>
-        <v>44</v>
+        <v>17</v>
       </c>
       <c r="J34" s="46">
         <f t="shared" ref="J34:AD34" si="1">SUM(J8:J33)</f>
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="K34" s="46">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="L34" s="46">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="M34" s="46">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="N34" s="46">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="O34" s="46">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="P34" s="46">
         <f t="shared" si="1"/>
@@ -4554,41 +4523,11 @@
       </c>
       <c r="AE34" s="45">
         <f>SUM(AE8:AE33)</f>
-        <v>110</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="B16:G16"/>
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="B12:G12"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B13:G13"/>
-    <mergeCell ref="B14:G14"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="B32:G32"/>
-    <mergeCell ref="B33:G33"/>
-    <mergeCell ref="B34:G34"/>
-    <mergeCell ref="B24:G24"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="B28:G28"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="B30:G30"/>
-    <mergeCell ref="B31:G31"/>
-    <mergeCell ref="A1:AE1"/>
-    <mergeCell ref="D2:AE2"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:O3"/>
     <mergeCell ref="B20:G20"/>
     <mergeCell ref="B21:G21"/>
     <mergeCell ref="B22:G22"/>
@@ -4605,6 +4544,36 @@
     <mergeCell ref="D5:F5"/>
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="B19:G19"/>
+    <mergeCell ref="A1:AE1"/>
+    <mergeCell ref="D2:AE2"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:O3"/>
+    <mergeCell ref="B32:G32"/>
+    <mergeCell ref="B33:G33"/>
+    <mergeCell ref="B34:G34"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="B30:G30"/>
+    <mergeCell ref="B31:G31"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B13:G13"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="B12:G12"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.61"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -4760,6 +4729,14 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_lisam_Description xmlns="6858a61b-99d0-4765-9cc3-c2f6eb1da4b6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -4768,22 +4745,14 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_lisam_Description xmlns="6858a61b-99d0-4765-9cc3-c2f6eb1da4b6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A512BC79-49A2-4FA0-A31D-8DDEDCFD05AC}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D77B6BA2-DAC6-4631-A24C-109FB1E3FCBF}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{791A3B54-D897-47E8-B515-70EBA147258E}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{791A3B54-D897-47E8-B515-70EBA147258E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D77B6BA2-DAC6-4631-A24C-109FB1E3FCBF}"/>
 </file>
</xml_diff>

<commit_message>
Made a layout design for the power circuitry
</commit_message>
<xml_diff>
--- a/docs/projektgrupp6_tidsplan.xlsx
+++ b/docs/projektgrupp6_tidsplan.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Documents\GitHub\CDIO\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\TNE085\git\CDIO\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61713055-3DC5-4A83-BC4E-FA2C0382FC14}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15375" windowHeight="5873" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15375" windowHeight="5880"/>
   </bookViews>
   <sheets>
     <sheet name="Basplan" sheetId="1" r:id="rId1"/>
     <sheet name="Summering TID" sheetId="5" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -204,7 +203,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -1092,129 +1091,20 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
@@ -1224,23 +1114,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1253,6 +1126,30 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
@@ -1261,11 +1158,180 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1275,73 +1341,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1627,130 +1626,130 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
       <selection activeCell="B23" sqref="B23:D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.1328125" customWidth="1"/>
-    <col min="2" max="2" width="18.1328125" customWidth="1"/>
-    <col min="3" max="3" width="9.1328125" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="3.140625" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="35" customWidth="1"/>
-    <col min="5" max="5" width="18.1328125" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="6.73046875" customWidth="1"/>
-    <col min="7" max="7" width="10.265625" customWidth="1"/>
-    <col min="8" max="30" width="2.73046875" customWidth="1"/>
-    <col min="31" max="31" width="3.73046875" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="6.7109375" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" customWidth="1"/>
+    <col min="8" max="30" width="2.7109375" customWidth="1"/>
+    <col min="31" max="31" width="3.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" s="15" customFormat="1" ht="17.649999999999999" x14ac:dyDescent="0.5">
-      <c r="A1" s="109" t="s">
+    <row r="1" spans="1:31" s="15" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A1" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="110"/>
-      <c r="C1" s="110"/>
-      <c r="D1" s="110"/>
-      <c r="E1" s="110"/>
-      <c r="F1" s="110"/>
-      <c r="G1" s="110"/>
-      <c r="H1" s="110"/>
-      <c r="I1" s="110"/>
-      <c r="J1" s="110"/>
-      <c r="K1" s="110"/>
-      <c r="L1" s="110"/>
-      <c r="M1" s="110"/>
-      <c r="N1" s="110"/>
-      <c r="O1" s="110"/>
-      <c r="P1" s="110"/>
-      <c r="Q1" s="110"/>
-      <c r="R1" s="110"/>
-      <c r="S1" s="110"/>
-      <c r="T1" s="110"/>
-      <c r="U1" s="110"/>
-      <c r="V1" s="110"/>
-      <c r="W1" s="110"/>
-      <c r="X1" s="110"/>
-      <c r="Y1" s="110"/>
-      <c r="Z1" s="110"/>
-      <c r="AA1" s="110"/>
-      <c r="AB1" s="110"/>
-      <c r="AC1" s="110"/>
-      <c r="AD1" s="110"/>
-      <c r="AE1" s="111"/>
-    </row>
-    <row r="2" spans="1:31" s="15" customFormat="1" ht="17.649999999999999" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="120" t="s">
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="73"/>
+      <c r="J1" s="73"/>
+      <c r="K1" s="73"/>
+      <c r="L1" s="73"/>
+      <c r="M1" s="73"/>
+      <c r="N1" s="73"/>
+      <c r="O1" s="73"/>
+      <c r="P1" s="73"/>
+      <c r="Q1" s="73"/>
+      <c r="R1" s="73"/>
+      <c r="S1" s="73"/>
+      <c r="T1" s="73"/>
+      <c r="U1" s="73"/>
+      <c r="V1" s="73"/>
+      <c r="W1" s="73"/>
+      <c r="X1" s="73"/>
+      <c r="Y1" s="73"/>
+      <c r="Z1" s="73"/>
+      <c r="AA1" s="73"/>
+      <c r="AB1" s="73"/>
+      <c r="AC1" s="73"/>
+      <c r="AD1" s="73"/>
+      <c r="AE1" s="74"/>
+    </row>
+    <row r="2" spans="1:31" s="15" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="93" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="121"/>
+      <c r="B2" s="94"/>
       <c r="C2" s="54"/>
-      <c r="D2" s="112" t="s">
+      <c r="D2" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="112"/>
-      <c r="F2" s="112"/>
-      <c r="G2" s="112"/>
-      <c r="H2" s="112"/>
-      <c r="I2" s="112"/>
-      <c r="J2" s="112"/>
-      <c r="K2" s="112"/>
-      <c r="L2" s="112"/>
-      <c r="M2" s="112"/>
-      <c r="N2" s="112"/>
-      <c r="O2" s="112"/>
-      <c r="P2" s="112"/>
-      <c r="Q2" s="112"/>
-      <c r="R2" s="112"/>
-      <c r="S2" s="112"/>
-      <c r="T2" s="112"/>
-      <c r="U2" s="112"/>
-      <c r="V2" s="112"/>
-      <c r="W2" s="112"/>
-      <c r="X2" s="112"/>
-      <c r="Y2" s="112"/>
-      <c r="Z2" s="112"/>
-      <c r="AA2" s="112"/>
-      <c r="AB2" s="112"/>
-      <c r="AC2" s="112"/>
-      <c r="AD2" s="112"/>
-      <c r="AE2" s="113"/>
-    </row>
-    <row r="3" spans="1:31" ht="15" x14ac:dyDescent="0.4">
-      <c r="A3" s="78" t="s">
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="75"/>
+      <c r="K2" s="75"/>
+      <c r="L2" s="75"/>
+      <c r="M2" s="75"/>
+      <c r="N2" s="75"/>
+      <c r="O2" s="75"/>
+      <c r="P2" s="75"/>
+      <c r="Q2" s="75"/>
+      <c r="R2" s="75"/>
+      <c r="S2" s="75"/>
+      <c r="T2" s="75"/>
+      <c r="U2" s="75"/>
+      <c r="V2" s="75"/>
+      <c r="W2" s="75"/>
+      <c r="X2" s="75"/>
+      <c r="Y2" s="75"/>
+      <c r="Z2" s="75"/>
+      <c r="AA2" s="75"/>
+      <c r="AB2" s="75"/>
+      <c r="AC2" s="75"/>
+      <c r="AD2" s="75"/>
+      <c r="AE2" s="76"/>
+    </row>
+    <row r="3" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="79"/>
+      <c r="B3" s="92"/>
       <c r="C3" s="13"/>
-      <c r="D3" s="92" t="s">
+      <c r="D3" s="97" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="92"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="78" t="s">
+      <c r="E3" s="97"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="91" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="79"/>
-      <c r="I3" s="84">
+      <c r="H3" s="92"/>
+      <c r="I3" s="116">
         <f ca="1">NOW()</f>
-        <v>43377.942739351849</v>
-      </c>
-      <c r="J3" s="84"/>
-      <c r="K3" s="84"/>
-      <c r="L3" s="84"/>
-      <c r="M3" s="84"/>
-      <c r="N3" s="84"/>
-      <c r="O3" s="85"/>
-      <c r="P3" s="78" t="s">
+        <v>43389.605141666667</v>
+      </c>
+      <c r="J3" s="116"/>
+      <c r="K3" s="116"/>
+      <c r="L3" s="116"/>
+      <c r="M3" s="116"/>
+      <c r="N3" s="116"/>
+      <c r="O3" s="117"/>
+      <c r="P3" s="91" t="s">
         <v>6</v>
       </c>
-      <c r="Q3" s="79"/>
-      <c r="R3" s="79"/>
-      <c r="S3" s="79"/>
-      <c r="T3" s="79"/>
+      <c r="Q3" s="92"/>
+      <c r="R3" s="92"/>
+      <c r="S3" s="92"/>
+      <c r="T3" s="92"/>
       <c r="U3" s="5"/>
       <c r="V3" s="5"/>
       <c r="W3" s="5"/>
@@ -1763,30 +1762,30 @@
       <c r="AD3" s="5"/>
       <c r="AE3" s="4"/>
     </row>
-    <row r="4" spans="1:31" ht="15" x14ac:dyDescent="0.4">
-      <c r="A4" s="80" t="s">
+    <row r="4" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="105" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="81"/>
+      <c r="B4" s="106"/>
       <c r="C4" s="13"/>
-      <c r="D4" s="94" t="s">
+      <c r="D4" s="99" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="94"/>
-      <c r="F4" s="95"/>
-      <c r="G4" s="80" t="s">
+      <c r="E4" s="99"/>
+      <c r="F4" s="100"/>
+      <c r="G4" s="105" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="81"/>
-      <c r="I4" s="86">
+      <c r="H4" s="106"/>
+      <c r="I4" s="118">
         <v>1</v>
       </c>
-      <c r="J4" s="86"/>
-      <c r="K4" s="86"/>
-      <c r="L4" s="86"/>
-      <c r="M4" s="86"/>
-      <c r="N4" s="86"/>
-      <c r="O4" s="87"/>
+      <c r="J4" s="118"/>
+      <c r="K4" s="118"/>
+      <c r="L4" s="118"/>
+      <c r="M4" s="118"/>
+      <c r="N4" s="118"/>
+      <c r="O4" s="119"/>
       <c r="P4" s="3"/>
       <c r="Q4" s="14"/>
       <c r="R4" s="14"/>
@@ -1804,30 +1803,30 @@
       <c r="AD4" s="14"/>
       <c r="AE4" s="4"/>
     </row>
-    <row r="5" spans="1:31" ht="15.4" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="82" t="s">
+    <row r="5" spans="1:31" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="103" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="83"/>
+      <c r="B5" s="104"/>
       <c r="C5" s="6"/>
-      <c r="D5" s="96" t="s">
+      <c r="D5" s="101" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="96"/>
-      <c r="F5" s="97"/>
-      <c r="G5" s="82" t="s">
+      <c r="E5" s="101"/>
+      <c r="F5" s="102"/>
+      <c r="G5" s="103" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="83"/>
-      <c r="I5" s="88" t="s">
+      <c r="H5" s="104"/>
+      <c r="I5" s="120" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="88"/>
-      <c r="K5" s="88"/>
-      <c r="L5" s="88"/>
-      <c r="M5" s="88"/>
-      <c r="N5" s="88"/>
-      <c r="O5" s="89"/>
+      <c r="J5" s="120"/>
+      <c r="K5" s="120"/>
+      <c r="L5" s="120"/>
+      <c r="M5" s="120"/>
+      <c r="N5" s="120"/>
+      <c r="O5" s="121"/>
       <c r="P5" s="3"/>
       <c r="Q5" s="5"/>
       <c r="R5" s="5"/>
@@ -1845,13 +1844,13 @@
       <c r="AD5" s="5"/>
       <c r="AE5" s="4"/>
     </row>
-    <row r="6" spans="1:31" s="2" customFormat="1" ht="15.4" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="107" t="s">
+    <row r="6" spans="1:31" s="2" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="77" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="108"/>
-      <c r="C6" s="108"/>
-      <c r="D6" s="108"/>
+      <c r="B6" s="78"/>
+      <c r="C6" s="78"/>
+      <c r="D6" s="78"/>
       <c r="E6" s="1"/>
       <c r="F6" s="16" t="s">
         <v>15</v>
@@ -1859,42 +1858,42 @@
       <c r="G6" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="107" t="s">
+      <c r="H6" s="77" t="s">
         <v>17</v>
       </c>
-      <c r="I6" s="108"/>
-      <c r="J6" s="108"/>
-      <c r="K6" s="108"/>
-      <c r="L6" s="108"/>
-      <c r="M6" s="108"/>
-      <c r="N6" s="108"/>
-      <c r="O6" s="108"/>
-      <c r="P6" s="108"/>
-      <c r="Q6" s="108"/>
-      <c r="R6" s="108"/>
-      <c r="S6" s="108"/>
-      <c r="T6" s="108"/>
-      <c r="U6" s="108"/>
-      <c r="V6" s="108"/>
-      <c r="W6" s="108"/>
-      <c r="X6" s="108"/>
-      <c r="Y6" s="108"/>
-      <c r="Z6" s="108"/>
-      <c r="AA6" s="108"/>
-      <c r="AB6" s="108"/>
-      <c r="AC6" s="108"/>
-      <c r="AD6" s="108"/>
-      <c r="AE6" s="114"/>
-    </row>
-    <row r="7" spans="1:31" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I6" s="78"/>
+      <c r="J6" s="78"/>
+      <c r="K6" s="78"/>
+      <c r="L6" s="78"/>
+      <c r="M6" s="78"/>
+      <c r="N6" s="78"/>
+      <c r="O6" s="78"/>
+      <c r="P6" s="78"/>
+      <c r="Q6" s="78"/>
+      <c r="R6" s="78"/>
+      <c r="S6" s="78"/>
+      <c r="T6" s="78"/>
+      <c r="U6" s="78"/>
+      <c r="V6" s="78"/>
+      <c r="W6" s="78"/>
+      <c r="X6" s="78"/>
+      <c r="Y6" s="78"/>
+      <c r="Z6" s="78"/>
+      <c r="AA6" s="78"/>
+      <c r="AB6" s="78"/>
+      <c r="AC6" s="78"/>
+      <c r="AD6" s="78"/>
+      <c r="AE6" s="79"/>
+    </row>
+    <row r="7" spans="1:31" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="115" t="s">
+      <c r="B7" s="80" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="116"/>
-      <c r="D7" s="117"/>
+      <c r="C7" s="81"/>
+      <c r="D7" s="82"/>
       <c r="E7" s="8"/>
       <c r="F7" s="9" t="s">
         <v>20</v>
@@ -1973,15 +1972,15 @@
       </c>
       <c r="AE7" s="11"/>
     </row>
-    <row r="8" spans="1:31" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:31" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11">
         <v>1</v>
       </c>
-      <c r="B8" s="98" t="s">
+      <c r="B8" s="107" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="99"/>
-      <c r="D8" s="100"/>
+      <c r="C8" s="108"/>
+      <c r="D8" s="109"/>
       <c r="E8" s="18"/>
       <c r="F8" s="19">
         <v>20</v>
@@ -2014,15 +2013,15 @@
       <c r="AD8" s="36"/>
       <c r="AE8" s="53"/>
     </row>
-    <row r="9" spans="1:31" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:31" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
         <v>2</v>
       </c>
-      <c r="B9" s="101" t="s">
+      <c r="B9" s="86" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="102"/>
-      <c r="D9" s="103"/>
+      <c r="C9" s="87"/>
+      <c r="D9" s="88"/>
       <c r="E9" s="21"/>
       <c r="F9" s="22">
         <v>16</v>
@@ -2055,15 +2054,15 @@
       <c r="AD9" s="37"/>
       <c r="AE9" s="4"/>
     </row>
-    <row r="10" spans="1:31" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:31" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11">
         <v>3</v>
       </c>
-      <c r="B10" s="101" t="s">
+      <c r="B10" s="86" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="102"/>
-      <c r="D10" s="103"/>
+      <c r="C10" s="87"/>
+      <c r="D10" s="88"/>
       <c r="E10" s="21"/>
       <c r="F10" s="22">
         <v>8</v>
@@ -2096,15 +2095,15 @@
       <c r="AD10" s="37"/>
       <c r="AE10" s="4"/>
     </row>
-    <row r="11" spans="1:31" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:31" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
         <v>4</v>
       </c>
-      <c r="B11" s="101" t="s">
+      <c r="B11" s="86" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="102"/>
-      <c r="D11" s="103"/>
+      <c r="C11" s="87"/>
+      <c r="D11" s="88"/>
       <c r="E11" s="21"/>
       <c r="F11" s="22">
         <v>8</v>
@@ -2137,15 +2136,15 @@
       <c r="AD11" s="37"/>
       <c r="AE11" s="4"/>
     </row>
-    <row r="12" spans="1:31" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:31" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11">
         <v>5</v>
       </c>
-      <c r="B12" s="101" t="s">
+      <c r="B12" s="86" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="102"/>
-      <c r="D12" s="103"/>
+      <c r="C12" s="87"/>
+      <c r="D12" s="88"/>
       <c r="E12" s="21"/>
       <c r="F12" s="22">
         <v>8</v>
@@ -2178,15 +2177,15 @@
       <c r="AD12" s="37"/>
       <c r="AE12" s="4"/>
     </row>
-    <row r="13" spans="1:31" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:31" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
         <v>6</v>
       </c>
-      <c r="B13" s="101" t="s">
+      <c r="B13" s="86" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="102"/>
-      <c r="D13" s="103"/>
+      <c r="C13" s="87"/>
+      <c r="D13" s="88"/>
       <c r="E13" s="21"/>
       <c r="F13" s="22">
         <v>12</v>
@@ -2219,15 +2218,15 @@
       <c r="AD13" s="37"/>
       <c r="AE13" s="4"/>
     </row>
-    <row r="14" spans="1:31" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:31" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11">
         <v>7</v>
       </c>
-      <c r="B14" s="101" t="s">
+      <c r="B14" s="86" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="102"/>
-      <c r="D14" s="103"/>
+      <c r="C14" s="87"/>
+      <c r="D14" s="88"/>
       <c r="E14" s="21"/>
       <c r="F14" s="22">
         <v>24</v>
@@ -2260,15 +2259,15 @@
       <c r="AD14" s="37"/>
       <c r="AE14" s="4"/>
     </row>
-    <row r="15" spans="1:31" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:31" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="11">
         <v>8</v>
       </c>
-      <c r="B15" s="101" t="s">
+      <c r="B15" s="86" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="102"/>
-      <c r="D15" s="103"/>
+      <c r="C15" s="87"/>
+      <c r="D15" s="88"/>
       <c r="E15" s="21"/>
       <c r="F15" s="22">
         <v>40</v>
@@ -2301,15 +2300,15 @@
       <c r="AD15" s="37"/>
       <c r="AE15" s="4"/>
     </row>
-    <row r="16" spans="1:31" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:31" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="11">
         <v>9</v>
       </c>
-      <c r="B16" s="101" t="s">
+      <c r="B16" s="86" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="102"/>
-      <c r="D16" s="103"/>
+      <c r="C16" s="87"/>
+      <c r="D16" s="88"/>
       <c r="E16" s="21"/>
       <c r="F16" s="22">
         <v>8</v>
@@ -2342,15 +2341,15 @@
       <c r="AD16" s="37"/>
       <c r="AE16" s="4"/>
     </row>
-    <row r="17" spans="1:31" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:31" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="11">
         <v>10</v>
       </c>
-      <c r="B17" s="101" t="s">
+      <c r="B17" s="86" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="102"/>
-      <c r="D17" s="103"/>
+      <c r="C17" s="87"/>
+      <c r="D17" s="88"/>
       <c r="E17" s="21"/>
       <c r="F17" s="22">
         <v>2</v>
@@ -2383,15 +2382,15 @@
       <c r="AD17" s="37"/>
       <c r="AE17" s="4"/>
     </row>
-    <row r="18" spans="1:31" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:31" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
         <v>11</v>
       </c>
-      <c r="B18" s="101" t="s">
+      <c r="B18" s="86" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="102"/>
-      <c r="D18" s="103"/>
+      <c r="C18" s="87"/>
+      <c r="D18" s="88"/>
       <c r="E18" s="21"/>
       <c r="F18" s="22">
         <v>16</v>
@@ -2424,15 +2423,15 @@
       <c r="AD18" s="37"/>
       <c r="AE18" s="4"/>
     </row>
-    <row r="19" spans="1:31" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:31" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="11">
         <v>12</v>
       </c>
-      <c r="B19" s="72" t="s">
+      <c r="B19" s="83" t="s">
         <v>34</v>
       </c>
-      <c r="C19" s="118"/>
-      <c r="D19" s="119"/>
+      <c r="C19" s="89"/>
+      <c r="D19" s="90"/>
       <c r="E19" s="21"/>
       <c r="F19" s="22">
         <v>24</v>
@@ -2465,15 +2464,15 @@
       <c r="AD19" s="37"/>
       <c r="AE19" s="4"/>
     </row>
-    <row r="20" spans="1:31" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:31" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11">
         <v>13</v>
       </c>
-      <c r="B20" s="72" t="s">
+      <c r="B20" s="83" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="75"/>
-      <c r="D20" s="76"/>
+      <c r="C20" s="84"/>
+      <c r="D20" s="85"/>
       <c r="E20" s="21"/>
       <c r="F20" s="22">
         <v>40</v>
@@ -2506,15 +2505,15 @@
       <c r="AD20" s="37"/>
       <c r="AE20" s="4"/>
     </row>
-    <row r="21" spans="1:31" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:31" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="11">
         <v>14</v>
       </c>
-      <c r="B21" s="72" t="s">
+      <c r="B21" s="83" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="73"/>
-      <c r="D21" s="74"/>
+      <c r="C21" s="114"/>
+      <c r="D21" s="115"/>
       <c r="E21" s="21"/>
       <c r="F21" s="22">
         <v>112</v>
@@ -2547,15 +2546,15 @@
       <c r="AD21" s="37"/>
       <c r="AE21" s="4"/>
     </row>
-    <row r="22" spans="1:31" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:31" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11">
         <v>15</v>
       </c>
-      <c r="B22" s="72" t="s">
+      <c r="B22" s="83" t="s">
         <v>56</v>
       </c>
-      <c r="C22" s="73"/>
-      <c r="D22" s="74"/>
+      <c r="C22" s="114"/>
+      <c r="D22" s="115"/>
       <c r="E22" s="21"/>
       <c r="F22" s="57" t="s">
         <v>37</v>
@@ -2588,15 +2587,15 @@
       <c r="AD22" s="37"/>
       <c r="AE22" s="4"/>
     </row>
-    <row r="23" spans="1:31" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:31" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
         <v>16</v>
       </c>
-      <c r="B23" s="72" t="s">
+      <c r="B23" s="83" t="s">
         <v>38</v>
       </c>
-      <c r="C23" s="73"/>
-      <c r="D23" s="74"/>
+      <c r="C23" s="114"/>
+      <c r="D23" s="115"/>
       <c r="E23" s="21"/>
       <c r="F23" s="22">
         <v>64</v>
@@ -2629,11 +2628,11 @@
       <c r="AD23" s="37"/>
       <c r="AE23" s="4"/>
     </row>
-    <row r="24" spans="1:31" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:31" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="11"/>
-      <c r="B24" s="72"/>
-      <c r="C24" s="73"/>
-      <c r="D24" s="74"/>
+      <c r="B24" s="83"/>
+      <c r="C24" s="114"/>
+      <c r="D24" s="115"/>
       <c r="E24" s="21"/>
       <c r="F24" s="22"/>
       <c r="G24" s="32"/>
@@ -2662,15 +2661,15 @@
       <c r="AD24" s="37"/>
       <c r="AE24" s="4"/>
     </row>
-    <row r="25" spans="1:31" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:31" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
         <v>17</v>
       </c>
-      <c r="B25" s="72" t="s">
+      <c r="B25" s="83" t="s">
         <v>39</v>
       </c>
-      <c r="C25" s="75"/>
-      <c r="D25" s="76"/>
+      <c r="C25" s="84"/>
+      <c r="D25" s="85"/>
       <c r="E25" s="21"/>
       <c r="F25" s="19">
         <v>10</v>
@@ -2703,11 +2702,11 @@
       <c r="AD25" s="61"/>
       <c r="AE25" s="4"/>
     </row>
-    <row r="26" spans="1:31" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:31" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11"/>
-      <c r="B26" s="77"/>
-      <c r="C26" s="75"/>
-      <c r="D26" s="76"/>
+      <c r="B26" s="113"/>
+      <c r="C26" s="84"/>
+      <c r="D26" s="85"/>
       <c r="E26" s="27"/>
       <c r="F26" s="22"/>
       <c r="G26" s="32"/>
@@ -2736,15 +2735,15 @@
       <c r="AD26" s="37"/>
       <c r="AE26" s="4"/>
     </row>
-    <row r="27" spans="1:31" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:31" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
         <v>18</v>
       </c>
-      <c r="B27" s="72" t="s">
+      <c r="B27" s="83" t="s">
         <v>40</v>
       </c>
-      <c r="C27" s="75"/>
-      <c r="D27" s="76"/>
+      <c r="C27" s="84"/>
+      <c r="D27" s="85"/>
       <c r="E27" s="21"/>
       <c r="F27" s="22"/>
       <c r="G27" s="62" t="s">
@@ -2777,15 +2776,15 @@
       <c r="AD27" s="44"/>
       <c r="AE27" s="4"/>
     </row>
-    <row r="28" spans="1:31" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:31" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="11">
         <v>19</v>
       </c>
-      <c r="B28" s="77" t="s">
+      <c r="B28" s="113" t="s">
         <v>42</v>
       </c>
-      <c r="C28" s="73"/>
-      <c r="D28" s="74"/>
+      <c r="C28" s="114"/>
+      <c r="D28" s="115"/>
       <c r="E28" s="21"/>
       <c r="F28" s="22"/>
       <c r="G28" s="62" t="s">
@@ -2818,15 +2817,15 @@
       <c r="AD28" s="37"/>
       <c r="AE28" s="4"/>
     </row>
-    <row r="29" spans="1:31" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:31" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
         <v>20</v>
       </c>
-      <c r="B29" s="77" t="s">
+      <c r="B29" s="113" t="s">
         <v>43</v>
       </c>
-      <c r="C29" s="75"/>
-      <c r="D29" s="76"/>
+      <c r="C29" s="84"/>
+      <c r="D29" s="85"/>
       <c r="E29" s="21"/>
       <c r="F29" s="22"/>
       <c r="G29" s="62" t="s">
@@ -2859,15 +2858,15 @@
       <c r="AD29" s="37"/>
       <c r="AE29" s="4"/>
     </row>
-    <row r="30" spans="1:31" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:31" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="11">
         <v>21</v>
       </c>
-      <c r="B30" s="77" t="s">
+      <c r="B30" s="113" t="s">
         <v>44</v>
       </c>
-      <c r="C30" s="75"/>
-      <c r="D30" s="76"/>
+      <c r="C30" s="84"/>
+      <c r="D30" s="85"/>
       <c r="E30" s="21"/>
       <c r="F30" s="22"/>
       <c r="G30" s="62" t="s">
@@ -2900,15 +2899,15 @@
       <c r="AD30" s="37"/>
       <c r="AE30" s="4"/>
     </row>
-    <row r="31" spans="1:31" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:31" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
         <v>22</v>
       </c>
-      <c r="B31" s="77" t="s">
+      <c r="B31" s="113" t="s">
         <v>46</v>
       </c>
-      <c r="C31" s="75"/>
-      <c r="D31" s="76"/>
+      <c r="C31" s="84"/>
+      <c r="D31" s="85"/>
       <c r="E31" s="21"/>
       <c r="F31" s="22"/>
       <c r="G31" s="62" t="s">
@@ -2939,15 +2938,15 @@
       <c r="AD31" s="37"/>
       <c r="AE31" s="4"/>
     </row>
-    <row r="32" spans="1:31" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:31" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="11">
         <v>23</v>
       </c>
-      <c r="B32" s="72" t="s">
+      <c r="B32" s="83" t="s">
         <v>47</v>
       </c>
-      <c r="C32" s="75"/>
-      <c r="D32" s="76"/>
+      <c r="C32" s="84"/>
+      <c r="D32" s="85"/>
       <c r="E32" s="21"/>
       <c r="F32" s="22"/>
       <c r="G32" s="62" t="s">
@@ -2978,13 +2977,13 @@
       <c r="AD32" s="37"/>
       <c r="AE32" s="4"/>
     </row>
-    <row r="33" spans="1:31" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:31" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="11">
         <v>24</v>
       </c>
-      <c r="B33" s="104"/>
-      <c r="C33" s="105"/>
-      <c r="D33" s="106"/>
+      <c r="B33" s="110"/>
+      <c r="C33" s="111"/>
+      <c r="D33" s="112"/>
       <c r="E33" s="21"/>
       <c r="F33" s="41"/>
       <c r="G33" s="43"/>
@@ -3013,13 +3012,13 @@
       <c r="AD33" s="39"/>
       <c r="AE33" s="4"/>
     </row>
-    <row r="34" spans="1:31" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:31" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
-      <c r="B34" s="90" t="s">
+      <c r="B34" s="95" t="s">
         <v>48</v>
       </c>
-      <c r="C34" s="90"/>
-      <c r="D34" s="91"/>
+      <c r="C34" s="95"/>
+      <c r="D34" s="96"/>
       <c r="E34" s="48"/>
       <c r="F34" s="49">
         <f>SUM(F8:F33)</f>
@@ -3053,6 +3052,36 @@
     </row>
   </sheetData>
   <mergeCells count="46">
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I3:O3"/>
+    <mergeCell ref="I4:O4"/>
+    <mergeCell ref="I5:O5"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="B30:D30"/>
     <mergeCell ref="A1:AE1"/>
     <mergeCell ref="D2:AE2"/>
     <mergeCell ref="H6:AE6"/>
@@ -3069,36 +3098,6 @@
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="P3:T3"/>
     <mergeCell ref="A2:B2"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I3:O3"/>
-    <mergeCell ref="I4:O4"/>
-    <mergeCell ref="I5:O5"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B23:D23"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="0.98425196850393704" bottom="0.78740157480314965" header="0.51181102362204722" footer="0.51181102362204722"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3109,131 +3108,131 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE34"/>
   <sheetViews>
     <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.1328125" customWidth="1"/>
-    <col min="2" max="2" width="18.1328125" customWidth="1"/>
-    <col min="3" max="3" width="9.1328125" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="27.1328125" customWidth="1"/>
-    <col min="5" max="5" width="18.1328125" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="6.73046875" customWidth="1"/>
-    <col min="7" max="7" width="10.265625" customWidth="1"/>
-    <col min="8" max="30" width="2.73046875" customWidth="1"/>
-    <col min="31" max="31" width="3.86328125" customWidth="1"/>
+    <col min="1" max="1" width="3.140625" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="6.7109375" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" customWidth="1"/>
+    <col min="8" max="30" width="2.7109375" customWidth="1"/>
+    <col min="31" max="31" width="3.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" s="15" customFormat="1" ht="17.649999999999999" x14ac:dyDescent="0.5">
-      <c r="A1" s="125" t="s">
+    <row r="1" spans="1:31" s="15" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A1" s="130" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="126"/>
-      <c r="C1" s="126"/>
-      <c r="D1" s="126"/>
-      <c r="E1" s="126"/>
-      <c r="F1" s="126"/>
-      <c r="G1" s="126"/>
-      <c r="H1" s="126"/>
-      <c r="I1" s="126"/>
-      <c r="J1" s="126"/>
-      <c r="K1" s="126"/>
-      <c r="L1" s="126"/>
-      <c r="M1" s="126"/>
-      <c r="N1" s="126"/>
-      <c r="O1" s="126"/>
-      <c r="P1" s="126"/>
-      <c r="Q1" s="126"/>
-      <c r="R1" s="126"/>
-      <c r="S1" s="126"/>
-      <c r="T1" s="126"/>
-      <c r="U1" s="126"/>
-      <c r="V1" s="126"/>
-      <c r="W1" s="126"/>
-      <c r="X1" s="126"/>
-      <c r="Y1" s="126"/>
-      <c r="Z1" s="126"/>
-      <c r="AA1" s="126"/>
-      <c r="AB1" s="126"/>
-      <c r="AC1" s="126"/>
-      <c r="AD1" s="126"/>
-      <c r="AE1" s="127"/>
-    </row>
-    <row r="2" spans="1:31" s="15" customFormat="1" ht="17.649999999999999" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="131" t="s">
+      <c r="B1" s="131"/>
+      <c r="C1" s="131"/>
+      <c r="D1" s="131"/>
+      <c r="E1" s="131"/>
+      <c r="F1" s="131"/>
+      <c r="G1" s="131"/>
+      <c r="H1" s="131"/>
+      <c r="I1" s="131"/>
+      <c r="J1" s="131"/>
+      <c r="K1" s="131"/>
+      <c r="L1" s="131"/>
+      <c r="M1" s="131"/>
+      <c r="N1" s="131"/>
+      <c r="O1" s="131"/>
+      <c r="P1" s="131"/>
+      <c r="Q1" s="131"/>
+      <c r="R1" s="131"/>
+      <c r="S1" s="131"/>
+      <c r="T1" s="131"/>
+      <c r="U1" s="131"/>
+      <c r="V1" s="131"/>
+      <c r="W1" s="131"/>
+      <c r="X1" s="131"/>
+      <c r="Y1" s="131"/>
+      <c r="Z1" s="131"/>
+      <c r="AA1" s="131"/>
+      <c r="AB1" s="131"/>
+      <c r="AC1" s="131"/>
+      <c r="AD1" s="131"/>
+      <c r="AE1" s="132"/>
+    </row>
+    <row r="2" spans="1:31" s="15" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="136" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="132"/>
+      <c r="B2" s="137"/>
       <c r="C2" s="55"/>
-      <c r="D2" s="128" t="str">
+      <c r="D2" s="133" t="str">
         <f>Basplan!D2</f>
         <v>Deepoid AB CDIO</v>
       </c>
-      <c r="E2" s="128"/>
-      <c r="F2" s="128"/>
-      <c r="G2" s="129"/>
-      <c r="H2" s="129"/>
-      <c r="I2" s="129"/>
-      <c r="J2" s="129"/>
-      <c r="K2" s="129"/>
-      <c r="L2" s="129"/>
-      <c r="M2" s="129"/>
-      <c r="N2" s="129"/>
-      <c r="O2" s="129"/>
-      <c r="P2" s="129"/>
-      <c r="Q2" s="129"/>
-      <c r="R2" s="129"/>
-      <c r="S2" s="129"/>
-      <c r="T2" s="129"/>
-      <c r="U2" s="129"/>
-      <c r="V2" s="129"/>
-      <c r="W2" s="129"/>
-      <c r="X2" s="129"/>
-      <c r="Y2" s="129"/>
-      <c r="Z2" s="129"/>
-      <c r="AA2" s="129"/>
-      <c r="AB2" s="129"/>
-      <c r="AC2" s="129"/>
-      <c r="AD2" s="129"/>
-      <c r="AE2" s="130"/>
-    </row>
-    <row r="3" spans="1:31" ht="15" x14ac:dyDescent="0.4">
-      <c r="A3" s="78" t="s">
+      <c r="E2" s="133"/>
+      <c r="F2" s="133"/>
+      <c r="G2" s="134"/>
+      <c r="H2" s="134"/>
+      <c r="I2" s="134"/>
+      <c r="J2" s="134"/>
+      <c r="K2" s="134"/>
+      <c r="L2" s="134"/>
+      <c r="M2" s="134"/>
+      <c r="N2" s="134"/>
+      <c r="O2" s="134"/>
+      <c r="P2" s="134"/>
+      <c r="Q2" s="134"/>
+      <c r="R2" s="134"/>
+      <c r="S2" s="134"/>
+      <c r="T2" s="134"/>
+      <c r="U2" s="134"/>
+      <c r="V2" s="134"/>
+      <c r="W2" s="134"/>
+      <c r="X2" s="134"/>
+      <c r="Y2" s="134"/>
+      <c r="Z2" s="134"/>
+      <c r="AA2" s="134"/>
+      <c r="AB2" s="134"/>
+      <c r="AC2" s="134"/>
+      <c r="AD2" s="134"/>
+      <c r="AE2" s="135"/>
+    </row>
+    <row r="3" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="79"/>
+      <c r="B3" s="92"/>
       <c r="C3" s="56"/>
-      <c r="D3" s="133" t="str">
+      <c r="D3" s="138" t="str">
         <f>Basplan!D3</f>
         <v>Grupp 6</v>
       </c>
-      <c r="E3" s="133"/>
-      <c r="F3" s="134"/>
-      <c r="G3" s="79" t="s">
+      <c r="E3" s="138"/>
+      <c r="F3" s="139"/>
+      <c r="G3" s="92" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="79"/>
-      <c r="I3" s="84">
+      <c r="H3" s="92"/>
+      <c r="I3" s="116">
         <f ca="1">NOW()</f>
-        <v>43377.942739351849</v>
-      </c>
-      <c r="J3" s="84"/>
-      <c r="K3" s="84"/>
-      <c r="L3" s="84"/>
-      <c r="M3" s="84"/>
-      <c r="N3" s="84"/>
-      <c r="O3" s="85"/>
-      <c r="P3" s="78" t="s">
+        <v>43389.605141666667</v>
+      </c>
+      <c r="J3" s="116"/>
+      <c r="K3" s="116"/>
+      <c r="L3" s="116"/>
+      <c r="M3" s="116"/>
+      <c r="N3" s="116"/>
+      <c r="O3" s="117"/>
+      <c r="P3" s="91" t="s">
         <v>6</v>
       </c>
-      <c r="Q3" s="79"/>
-      <c r="R3" s="79"/>
-      <c r="S3" s="79"/>
+      <c r="Q3" s="92"/>
+      <c r="R3" s="92"/>
+      <c r="S3" s="92"/>
       <c r="T3" s="5"/>
       <c r="U3" s="5"/>
       <c r="V3" s="5"/>
@@ -3247,31 +3246,31 @@
       <c r="AD3" s="5"/>
       <c r="AE3" s="4"/>
     </row>
-    <row r="4" spans="1:31" ht="15" x14ac:dyDescent="0.4">
-      <c r="A4" s="80" t="s">
+    <row r="4" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="105" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="81"/>
+      <c r="B4" s="106"/>
       <c r="C4" s="13"/>
-      <c r="D4" s="86" t="str">
+      <c r="D4" s="118" t="str">
         <f>Basplan!D4</f>
         <v>Deepoid AB</v>
       </c>
-      <c r="E4" s="86"/>
-      <c r="F4" s="87"/>
-      <c r="G4" s="81" t="s">
+      <c r="E4" s="118"/>
+      <c r="F4" s="119"/>
+      <c r="G4" s="106" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="81"/>
-      <c r="I4" s="86">
+      <c r="H4" s="106"/>
+      <c r="I4" s="118">
         <v>1</v>
       </c>
-      <c r="J4" s="86"/>
-      <c r="K4" s="86"/>
-      <c r="L4" s="86"/>
-      <c r="M4" s="86"/>
-      <c r="N4" s="86"/>
-      <c r="O4" s="87"/>
+      <c r="J4" s="118"/>
+      <c r="K4" s="118"/>
+      <c r="L4" s="118"/>
+      <c r="M4" s="118"/>
+      <c r="N4" s="118"/>
+      <c r="O4" s="119"/>
       <c r="P4" s="3"/>
       <c r="Q4" s="14"/>
       <c r="R4" s="14"/>
@@ -3289,31 +3288,31 @@
       <c r="AD4" s="14"/>
       <c r="AE4" s="4"/>
     </row>
-    <row r="5" spans="1:31" ht="15.4" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="82" t="s">
+    <row r="5" spans="1:31" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="103" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="83"/>
+      <c r="B5" s="104"/>
       <c r="C5" s="6"/>
-      <c r="D5" s="88" t="str">
+      <c r="D5" s="120" t="str">
         <f>Basplan!D5</f>
         <v>CDIO</v>
       </c>
-      <c r="E5" s="88"/>
-      <c r="F5" s="89"/>
-      <c r="G5" s="83" t="s">
+      <c r="E5" s="120"/>
+      <c r="F5" s="121"/>
+      <c r="G5" s="104" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="83"/>
-      <c r="I5" s="88" t="s">
+      <c r="H5" s="104"/>
+      <c r="I5" s="120" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="88"/>
-      <c r="K5" s="88"/>
-      <c r="L5" s="88"/>
-      <c r="M5" s="88"/>
-      <c r="N5" s="88"/>
-      <c r="O5" s="89"/>
+      <c r="J5" s="120"/>
+      <c r="K5" s="120"/>
+      <c r="L5" s="120"/>
+      <c r="M5" s="120"/>
+      <c r="N5" s="120"/>
+      <c r="O5" s="121"/>
       <c r="P5" s="3"/>
       <c r="Q5" s="5"/>
       <c r="R5" s="5"/>
@@ -3331,53 +3330,53 @@
       <c r="AD5" s="5"/>
       <c r="AE5" s="4"/>
     </row>
-    <row r="6" spans="1:31" s="2" customFormat="1" ht="15.4" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="122" t="s">
+    <row r="6" spans="1:31" s="2" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="140" t="s">
         <v>50</v>
       </c>
-      <c r="B6" s="123"/>
-      <c r="C6" s="123"/>
-      <c r="D6" s="123"/>
-      <c r="E6" s="123"/>
-      <c r="F6" s="123"/>
-      <c r="G6" s="124"/>
-      <c r="H6" s="107" t="s">
+      <c r="B6" s="141"/>
+      <c r="C6" s="141"/>
+      <c r="D6" s="141"/>
+      <c r="E6" s="141"/>
+      <c r="F6" s="141"/>
+      <c r="G6" s="142"/>
+      <c r="H6" s="77" t="s">
         <v>51</v>
       </c>
-      <c r="I6" s="108"/>
-      <c r="J6" s="108"/>
-      <c r="K6" s="108"/>
-      <c r="L6" s="108"/>
-      <c r="M6" s="108"/>
-      <c r="N6" s="108"/>
-      <c r="O6" s="108"/>
-      <c r="P6" s="108"/>
-      <c r="Q6" s="108"/>
-      <c r="R6" s="108"/>
-      <c r="S6" s="108"/>
-      <c r="T6" s="108"/>
-      <c r="U6" s="108"/>
-      <c r="V6" s="108"/>
-      <c r="W6" s="108"/>
-      <c r="X6" s="108"/>
-      <c r="Y6" s="108"/>
-      <c r="Z6" s="108"/>
-      <c r="AA6" s="108"/>
-      <c r="AB6" s="108"/>
-      <c r="AC6" s="108"/>
-      <c r="AD6" s="108"/>
-      <c r="AE6" s="114"/>
-    </row>
-    <row r="7" spans="1:31" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I6" s="78"/>
+      <c r="J6" s="78"/>
+      <c r="K6" s="78"/>
+      <c r="L6" s="78"/>
+      <c r="M6" s="78"/>
+      <c r="N6" s="78"/>
+      <c r="O6" s="78"/>
+      <c r="P6" s="78"/>
+      <c r="Q6" s="78"/>
+      <c r="R6" s="78"/>
+      <c r="S6" s="78"/>
+      <c r="T6" s="78"/>
+      <c r="U6" s="78"/>
+      <c r="V6" s="78"/>
+      <c r="W6" s="78"/>
+      <c r="X6" s="78"/>
+      <c r="Y6" s="78"/>
+      <c r="Z6" s="78"/>
+      <c r="AA6" s="78"/>
+      <c r="AB6" s="78"/>
+      <c r="AC6" s="78"/>
+      <c r="AD6" s="78"/>
+      <c r="AE6" s="79"/>
+    </row>
+    <row r="7" spans="1:31" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
-      <c r="B7" s="115" t="s">
+      <c r="B7" s="80" t="s">
         <v>52</v>
       </c>
-      <c r="C7" s="116"/>
-      <c r="D7" s="116"/>
-      <c r="E7" s="116"/>
-      <c r="F7" s="116"/>
-      <c r="G7" s="117"/>
+      <c r="C7" s="81"/>
+      <c r="D7" s="81"/>
+      <c r="E7" s="81"/>
+      <c r="F7" s="81"/>
+      <c r="G7" s="82"/>
       <c r="H7" s="35">
         <f>Basplan!H7</f>
         <v>36</v>
@@ -3474,16 +3473,16 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A8" s="12"/>
-      <c r="B8" s="140" t="s">
+      <c r="B8" s="122" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="141"/>
-      <c r="D8" s="141"/>
-      <c r="E8" s="141"/>
-      <c r="F8" s="141"/>
-      <c r="G8" s="142"/>
+      <c r="C8" s="123"/>
+      <c r="D8" s="123"/>
+      <c r="E8" s="123"/>
+      <c r="F8" s="123"/>
+      <c r="G8" s="124"/>
       <c r="H8" s="30">
         <v>12</v>
       </c>
@@ -3499,7 +3498,9 @@
       <c r="L8" s="20">
         <v>20</v>
       </c>
-      <c r="M8" s="20"/>
+      <c r="M8" s="20">
+        <v>24</v>
+      </c>
       <c r="N8" s="20"/>
       <c r="O8" s="20"/>
       <c r="P8" s="20"/>
@@ -3519,19 +3520,19 @@
       <c r="AD8" s="36"/>
       <c r="AE8" s="33">
         <f t="shared" ref="AE8:AE33" si="0">SUM(H8:AD8)</f>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.35">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A9" s="12"/>
-      <c r="B9" s="77" t="s">
+      <c r="B9" s="113" t="s">
         <v>54</v>
       </c>
-      <c r="C9" s="75"/>
-      <c r="D9" s="75"/>
-      <c r="E9" s="75"/>
-      <c r="F9" s="75"/>
-      <c r="G9" s="76"/>
+      <c r="C9" s="84"/>
+      <c r="D9" s="84"/>
+      <c r="E9" s="84"/>
+      <c r="F9" s="84"/>
+      <c r="G9" s="85"/>
       <c r="H9" s="23">
         <v>10</v>
       </c>
@@ -3568,14 +3569,14 @@
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A10" s="12"/>
-      <c r="B10" s="77"/>
-      <c r="C10" s="75"/>
-      <c r="D10" s="75"/>
-      <c r="E10" s="75"/>
-      <c r="F10" s="75"/>
-      <c r="G10" s="76"/>
+      <c r="B10" s="113"/>
+      <c r="C10" s="84"/>
+      <c r="D10" s="84"/>
+      <c r="E10" s="84"/>
+      <c r="F10" s="84"/>
+      <c r="G10" s="85"/>
       <c r="H10" s="23"/>
       <c r="I10" s="24"/>
       <c r="J10" s="24"/>
@@ -3604,14 +3605,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A11" s="12"/>
-      <c r="B11" s="77"/>
-      <c r="C11" s="75"/>
-      <c r="D11" s="75"/>
-      <c r="E11" s="75"/>
-      <c r="F11" s="75"/>
-      <c r="G11" s="76"/>
+      <c r="B11" s="113"/>
+      <c r="C11" s="84"/>
+      <c r="D11" s="84"/>
+      <c r="E11" s="84"/>
+      <c r="F11" s="84"/>
+      <c r="G11" s="85"/>
       <c r="H11" s="23"/>
       <c r="I11" s="24"/>
       <c r="J11" s="24"/>
@@ -3640,14 +3641,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A12" s="12"/>
-      <c r="B12" s="77"/>
-      <c r="C12" s="75"/>
-      <c r="D12" s="75"/>
-      <c r="E12" s="75"/>
-      <c r="F12" s="75"/>
-      <c r="G12" s="76"/>
+      <c r="B12" s="113"/>
+      <c r="C12" s="84"/>
+      <c r="D12" s="84"/>
+      <c r="E12" s="84"/>
+      <c r="F12" s="84"/>
+      <c r="G12" s="85"/>
       <c r="H12" s="23"/>
       <c r="I12" s="24"/>
       <c r="J12" s="24"/>
@@ -3676,14 +3677,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
-      <c r="B13" s="77"/>
-      <c r="C13" s="75"/>
-      <c r="D13" s="75"/>
-      <c r="E13" s="75"/>
-      <c r="F13" s="75"/>
-      <c r="G13" s="76"/>
+      <c r="B13" s="113"/>
+      <c r="C13" s="84"/>
+      <c r="D13" s="84"/>
+      <c r="E13" s="84"/>
+      <c r="F13" s="84"/>
+      <c r="G13" s="85"/>
       <c r="H13" s="23"/>
       <c r="I13" s="24"/>
       <c r="J13" s="24"/>
@@ -3712,14 +3713,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A14" s="12"/>
-      <c r="B14" s="77"/>
-      <c r="C14" s="75"/>
-      <c r="D14" s="75"/>
-      <c r="E14" s="75"/>
-      <c r="F14" s="75"/>
-      <c r="G14" s="76"/>
+      <c r="B14" s="113"/>
+      <c r="C14" s="84"/>
+      <c r="D14" s="84"/>
+      <c r="E14" s="84"/>
+      <c r="F14" s="84"/>
+      <c r="G14" s="85"/>
       <c r="H14" s="23"/>
       <c r="I14" s="24"/>
       <c r="J14" s="24"/>
@@ -3748,14 +3749,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A15" s="12"/>
-      <c r="B15" s="77"/>
-      <c r="C15" s="75"/>
-      <c r="D15" s="75"/>
-      <c r="E15" s="75"/>
-      <c r="F15" s="75"/>
-      <c r="G15" s="76"/>
+      <c r="B15" s="113"/>
+      <c r="C15" s="84"/>
+      <c r="D15" s="84"/>
+      <c r="E15" s="84"/>
+      <c r="F15" s="84"/>
+      <c r="G15" s="85"/>
       <c r="H15" s="23"/>
       <c r="I15" s="24"/>
       <c r="J15" s="24"/>
@@ -3784,14 +3785,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A16" s="12"/>
-      <c r="B16" s="77"/>
-      <c r="C16" s="75"/>
-      <c r="D16" s="75"/>
-      <c r="E16" s="75"/>
-      <c r="F16" s="75"/>
-      <c r="G16" s="76"/>
+      <c r="B16" s="113"/>
+      <c r="C16" s="84"/>
+      <c r="D16" s="84"/>
+      <c r="E16" s="84"/>
+      <c r="F16" s="84"/>
+      <c r="G16" s="85"/>
       <c r="H16" s="23"/>
       <c r="I16" s="24"/>
       <c r="J16" s="24"/>
@@ -3820,14 +3821,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A17" s="12"/>
-      <c r="B17" s="77"/>
-      <c r="C17" s="75"/>
-      <c r="D17" s="75"/>
-      <c r="E17" s="75"/>
-      <c r="F17" s="75"/>
-      <c r="G17" s="76"/>
+      <c r="B17" s="113"/>
+      <c r="C17" s="84"/>
+      <c r="D17" s="84"/>
+      <c r="E17" s="84"/>
+      <c r="F17" s="84"/>
+      <c r="G17" s="85"/>
       <c r="H17" s="23"/>
       <c r="I17" s="24"/>
       <c r="J17" s="24"/>
@@ -3856,14 +3857,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A18" s="12"/>
-      <c r="B18" s="77"/>
-      <c r="C18" s="75"/>
-      <c r="D18" s="75"/>
-      <c r="E18" s="75"/>
-      <c r="F18" s="75"/>
-      <c r="G18" s="76"/>
+      <c r="B18" s="113"/>
+      <c r="C18" s="84"/>
+      <c r="D18" s="84"/>
+      <c r="E18" s="84"/>
+      <c r="F18" s="84"/>
+      <c r="G18" s="85"/>
       <c r="H18" s="23"/>
       <c r="I18" s="24"/>
       <c r="J18" s="24"/>
@@ -3892,14 +3893,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A19" s="12"/>
-      <c r="B19" s="77"/>
-      <c r="C19" s="75"/>
-      <c r="D19" s="75"/>
-      <c r="E19" s="75"/>
-      <c r="F19" s="75"/>
-      <c r="G19" s="76"/>
+      <c r="B19" s="113"/>
+      <c r="C19" s="84"/>
+      <c r="D19" s="84"/>
+      <c r="E19" s="84"/>
+      <c r="F19" s="84"/>
+      <c r="G19" s="85"/>
       <c r="H19" s="23"/>
       <c r="I19" s="24"/>
       <c r="J19" s="24"/>
@@ -3928,14 +3929,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A20" s="12"/>
-      <c r="B20" s="77"/>
-      <c r="C20" s="75"/>
-      <c r="D20" s="75"/>
-      <c r="E20" s="75"/>
-      <c r="F20" s="75"/>
-      <c r="G20" s="76"/>
+      <c r="B20" s="113"/>
+      <c r="C20" s="84"/>
+      <c r="D20" s="84"/>
+      <c r="E20" s="84"/>
+      <c r="F20" s="84"/>
+      <c r="G20" s="85"/>
       <c r="H20" s="23"/>
       <c r="I20" s="24"/>
       <c r="J20" s="24"/>
@@ -3964,14 +3965,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A21" s="12"/>
-      <c r="B21" s="77"/>
-      <c r="C21" s="75"/>
-      <c r="D21" s="75"/>
-      <c r="E21" s="75"/>
-      <c r="F21" s="75"/>
-      <c r="G21" s="76"/>
+      <c r="B21" s="113"/>
+      <c r="C21" s="84"/>
+      <c r="D21" s="84"/>
+      <c r="E21" s="84"/>
+      <c r="F21" s="84"/>
+      <c r="G21" s="85"/>
       <c r="H21" s="23"/>
       <c r="I21" s="24"/>
       <c r="J21" s="24"/>
@@ -4000,14 +4001,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A22" s="12"/>
-      <c r="B22" s="77"/>
-      <c r="C22" s="75"/>
-      <c r="D22" s="75"/>
-      <c r="E22" s="75"/>
-      <c r="F22" s="75"/>
-      <c r="G22" s="76"/>
+      <c r="B22" s="113"/>
+      <c r="C22" s="84"/>
+      <c r="D22" s="84"/>
+      <c r="E22" s="84"/>
+      <c r="F22" s="84"/>
+      <c r="G22" s="85"/>
       <c r="H22" s="23"/>
       <c r="I22" s="24"/>
       <c r="J22" s="24"/>
@@ -4036,14 +4037,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A23" s="12"/>
-      <c r="B23" s="77"/>
-      <c r="C23" s="75"/>
-      <c r="D23" s="75"/>
-      <c r="E23" s="75"/>
-      <c r="F23" s="75"/>
-      <c r="G23" s="76"/>
+      <c r="B23" s="113"/>
+      <c r="C23" s="84"/>
+      <c r="D23" s="84"/>
+      <c r="E23" s="84"/>
+      <c r="F23" s="84"/>
+      <c r="G23" s="85"/>
       <c r="H23" s="23"/>
       <c r="I23" s="24"/>
       <c r="J23" s="24"/>
@@ -4072,14 +4073,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A24" s="12"/>
-      <c r="B24" s="77"/>
-      <c r="C24" s="75"/>
-      <c r="D24" s="75"/>
-      <c r="E24" s="75"/>
-      <c r="F24" s="75"/>
-      <c r="G24" s="76"/>
+      <c r="B24" s="113"/>
+      <c r="C24" s="84"/>
+      <c r="D24" s="84"/>
+      <c r="E24" s="84"/>
+      <c r="F24" s="84"/>
+      <c r="G24" s="85"/>
       <c r="H24" s="23"/>
       <c r="I24" s="24"/>
       <c r="J24" s="24"/>
@@ -4108,14 +4109,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A25" s="12"/>
-      <c r="B25" s="77"/>
-      <c r="C25" s="75"/>
-      <c r="D25" s="75"/>
-      <c r="E25" s="75"/>
-      <c r="F25" s="75"/>
-      <c r="G25" s="76"/>
+      <c r="B25" s="113"/>
+      <c r="C25" s="84"/>
+      <c r="D25" s="84"/>
+      <c r="E25" s="84"/>
+      <c r="F25" s="84"/>
+      <c r="G25" s="85"/>
       <c r="H25" s="23"/>
       <c r="I25" s="24"/>
       <c r="J25" s="24"/>
@@ -4144,14 +4145,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A26" s="12"/>
-      <c r="B26" s="77"/>
-      <c r="C26" s="75"/>
-      <c r="D26" s="75"/>
-      <c r="E26" s="75"/>
-      <c r="F26" s="75"/>
-      <c r="G26" s="76"/>
+      <c r="B26" s="113"/>
+      <c r="C26" s="84"/>
+      <c r="D26" s="84"/>
+      <c r="E26" s="84"/>
+      <c r="F26" s="84"/>
+      <c r="G26" s="85"/>
       <c r="H26" s="23"/>
       <c r="I26" s="24"/>
       <c r="J26" s="24"/>
@@ -4180,14 +4181,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A27" s="12"/>
-      <c r="B27" s="77"/>
-      <c r="C27" s="75"/>
-      <c r="D27" s="75"/>
-      <c r="E27" s="75"/>
-      <c r="F27" s="75"/>
-      <c r="G27" s="76"/>
+      <c r="B27" s="113"/>
+      <c r="C27" s="84"/>
+      <c r="D27" s="84"/>
+      <c r="E27" s="84"/>
+      <c r="F27" s="84"/>
+      <c r="G27" s="85"/>
       <c r="H27" s="23"/>
       <c r="I27" s="24"/>
       <c r="J27" s="24"/>
@@ -4216,14 +4217,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A28" s="42"/>
-      <c r="B28" s="77"/>
-      <c r="C28" s="75"/>
-      <c r="D28" s="75"/>
-      <c r="E28" s="75"/>
-      <c r="F28" s="75"/>
-      <c r="G28" s="76"/>
+      <c r="B28" s="113"/>
+      <c r="C28" s="84"/>
+      <c r="D28" s="84"/>
+      <c r="E28" s="84"/>
+      <c r="F28" s="84"/>
+      <c r="G28" s="85"/>
       <c r="H28" s="23"/>
       <c r="I28" s="24"/>
       <c r="J28" s="24"/>
@@ -4252,14 +4253,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A29" s="42"/>
-      <c r="B29" s="77"/>
-      <c r="C29" s="75"/>
-      <c r="D29" s="75"/>
-      <c r="E29" s="75"/>
-      <c r="F29" s="75"/>
-      <c r="G29" s="76"/>
+      <c r="B29" s="113"/>
+      <c r="C29" s="84"/>
+      <c r="D29" s="84"/>
+      <c r="E29" s="84"/>
+      <c r="F29" s="84"/>
+      <c r="G29" s="85"/>
       <c r="H29" s="23"/>
       <c r="I29" s="24"/>
       <c r="J29" s="24"/>
@@ -4288,14 +4289,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A30" s="12"/>
-      <c r="B30" s="77"/>
-      <c r="C30" s="75"/>
-      <c r="D30" s="75"/>
-      <c r="E30" s="75"/>
-      <c r="F30" s="75"/>
-      <c r="G30" s="76"/>
+      <c r="B30" s="113"/>
+      <c r="C30" s="84"/>
+      <c r="D30" s="84"/>
+      <c r="E30" s="84"/>
+      <c r="F30" s="84"/>
+      <c r="G30" s="85"/>
       <c r="H30" s="23"/>
       <c r="I30" s="24"/>
       <c r="J30" s="24"/>
@@ -4324,14 +4325,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A31" s="12"/>
-      <c r="B31" s="77"/>
-      <c r="C31" s="75"/>
-      <c r="D31" s="75"/>
-      <c r="E31" s="75"/>
-      <c r="F31" s="75"/>
-      <c r="G31" s="76"/>
+      <c r="B31" s="113"/>
+      <c r="C31" s="84"/>
+      <c r="D31" s="84"/>
+      <c r="E31" s="84"/>
+      <c r="F31" s="84"/>
+      <c r="G31" s="85"/>
       <c r="H31" s="23"/>
       <c r="I31" s="24"/>
       <c r="J31" s="24"/>
@@ -4360,14 +4361,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A32" s="12"/>
-      <c r="B32" s="77"/>
-      <c r="C32" s="75"/>
-      <c r="D32" s="75"/>
-      <c r="E32" s="75"/>
-      <c r="F32" s="75"/>
-      <c r="G32" s="76"/>
+      <c r="B32" s="113"/>
+      <c r="C32" s="84"/>
+      <c r="D32" s="84"/>
+      <c r="E32" s="84"/>
+      <c r="F32" s="84"/>
+      <c r="G32" s="85"/>
       <c r="H32" s="23"/>
       <c r="I32" s="24"/>
       <c r="J32" s="24"/>
@@ -4396,14 +4397,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:31" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:31" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="12"/>
-      <c r="B33" s="135"/>
-      <c r="C33" s="136"/>
-      <c r="D33" s="136"/>
-      <c r="E33" s="136"/>
-      <c r="F33" s="136"/>
-      <c r="G33" s="137"/>
+      <c r="B33" s="125"/>
+      <c r="C33" s="126"/>
+      <c r="D33" s="126"/>
+      <c r="E33" s="126"/>
+      <c r="F33" s="126"/>
+      <c r="G33" s="127"/>
       <c r="H33" s="38"/>
       <c r="I33" s="26"/>
       <c r="J33" s="26"/>
@@ -4432,16 +4433,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:31" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:31" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="9"/>
-      <c r="B34" s="138" t="s">
+      <c r="B34" s="128" t="s">
         <v>55</v>
       </c>
-      <c r="C34" s="138"/>
-      <c r="D34" s="138"/>
-      <c r="E34" s="138"/>
-      <c r="F34" s="138"/>
-      <c r="G34" s="139"/>
+      <c r="C34" s="128"/>
+      <c r="D34" s="128"/>
+      <c r="E34" s="128"/>
+      <c r="F34" s="128"/>
+      <c r="G34" s="129"/>
       <c r="H34" s="40">
         <f>SUM(H8:H33)</f>
         <v>22</v>
@@ -4464,7 +4465,7 @@
       </c>
       <c r="M34" s="46">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="N34" s="46">
         <f t="shared" si="1"/>
@@ -4536,41 +4537,11 @@
       </c>
       <c r="AE34" s="45">
         <f>SUM(AE8:AE33)</f>
-        <v>138</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="B16:G16"/>
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="B12:G12"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B13:G13"/>
-    <mergeCell ref="B14:G14"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="B32:G32"/>
-    <mergeCell ref="B33:G33"/>
-    <mergeCell ref="B34:G34"/>
-    <mergeCell ref="B24:G24"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="B28:G28"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="B30:G30"/>
-    <mergeCell ref="B31:G31"/>
-    <mergeCell ref="A1:AE1"/>
-    <mergeCell ref="D2:AE2"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:O3"/>
     <mergeCell ref="B20:G20"/>
     <mergeCell ref="B21:G21"/>
     <mergeCell ref="B22:G22"/>
@@ -4587,6 +4558,36 @@
     <mergeCell ref="D5:F5"/>
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="B19:G19"/>
+    <mergeCell ref="A1:AE1"/>
+    <mergeCell ref="D2:AE2"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:O3"/>
+    <mergeCell ref="B32:G32"/>
+    <mergeCell ref="B33:G33"/>
+    <mergeCell ref="B34:G34"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="B30:G30"/>
+    <mergeCell ref="B31:G31"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B13:G13"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="B12:G12"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.61"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -4597,23 +4598,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_lisam_Description xmlns="6858a61b-99d0-4765-9cc3-c2f6eb1da4b6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="dokument" ma:contentTypeID="0x01010013D783E7FF902C40B92D449D6BECD3AB" ma:contentTypeVersion="3" ma:contentTypeDescription="Skapa ett nytt dokument." ma:contentTypeScope="" ma:versionID="fe8eabd614b2bd4c9f8424f9fb111368">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6858a61b-99d0-4765-9cc3-c2f6eb1da4b6" xmlns:ns3="ed6ba336-f2c3-44c7-9b01-7d62384a4ed8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a5bf6526ec41d69fe6df6b959e7fb77f" ns2:_="" ns3:_="">
     <xsd:import namespace="6858a61b-99d0-4765-9cc3-c2f6eb1da4b6"/>
@@ -4758,25 +4742,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D77B6BA2-DAC6-4631-A24C-109FB1E3FCBF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_lisam_Description xmlns="6858a61b-99d0-4765-9cc3-c2f6eb1da4b6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{791A3B54-D897-47E8-B515-70EBA147258E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="6858a61b-99d0-4765-9cc3-c2f6eb1da4b6"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A512BC79-49A2-4FA0-A31D-8DDEDCFD05AC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4793,4 +4776,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{791A3B54-D897-47E8-B515-70EBA147258E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="6858a61b-99d0-4765-9cc3-c2f6eb1da4b6"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D77B6BA2-DAC6-4631-A24C-109FB1E3FCBF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>